<commit_message>
Pflichtenheft überarbeitet & Recherche
</commit_message>
<xml_diff>
--- a/Dokumente/20240913_Zeitplan.xlsx
+++ b/Dokumente/20240913_Zeitplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c9cb578a977eee7/Desktop/project/diplomarbeit/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:1_{4E4E044E-0397-49A1-8B73-67D9B76A8147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C64EFA3-9664-4F66-8D0C-323D05693019}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="13_ncr:1_{4E4E044E-0397-49A1-8B73-67D9B76A8147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F373FE9-AB88-4047-A864-A1357650E366}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12649" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -652,16 +652,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1055,67 +1055,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>397112</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>54982</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>397111</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>145439</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Grafik 11" descr="MongoDB logo | Infinapps">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09EB86FA-3635-4F18-C62C-98B9B8633F97}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5287846" y="243088"/>
-          <a:ext cx="1630244" cy="1971508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>606117</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -1141,7 +1080,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1202,7 +1141,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1263,7 +1202,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1324,7 +1263,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1481,7 +1420,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1497,6 +1436,67 @@
         <a:xfrm>
           <a:off x="10105426" y="2821577"/>
           <a:ext cx="1853967" cy="1912402"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>156755</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>156755</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>693098</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>84273</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32630988-4F6A-5604-50DE-EC4AA1C9FBF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5047489" y="532965"/>
+          <a:ext cx="2166588" cy="1808569"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1807,56 +1807,56 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="38" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="38" t="s">
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="38" t="s">
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="38" t="s">
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="38" t="s">
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="38" t="s">
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="38" t="s">
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="AH1" s="40"/>
+      <c r="AH1" s="38"/>
     </row>
     <row r="2" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
@@ -1999,8 +1999,8 @@
         <v>4</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="37"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="40"/>
       <c r="AH5" s="14"/>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.3">
@@ -3331,16 +3331,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="T1:X1"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3351,8 +3351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CAAB76-81FF-479D-9151-CB58DF96AA0A}">
   <dimension ref="A1:AG110"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4297,7 +4297,6 @@
       <c r="N27" s="27"/>
       <c r="O27" s="28"/>
       <c r="P27" s="32"/>
-      <c r="Q27" s="32"/>
       <c r="R27" s="32"/>
       <c r="S27" s="32"/>
       <c r="T27" s="32"/>
@@ -5251,7 +5250,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5351,7 +5350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3496E6-DAA5-470E-A81E-AE446E442BDE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Präsentation 1 Diagramme & CO
</commit_message>
<xml_diff>
--- a/Dokumente/20240913_Zeitplan.xlsx
+++ b/Dokumente/20240913_Zeitplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c9cb578a977eee7/Desktop/project/diplomarbeit/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="298" documentId="13_ncr:1_{4E4E044E-0397-49A1-8B73-67D9B76A8147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F165A207-7739-4203-8BBB-53E32CF9C873}"/>
+  <xr:revisionPtr revIDLastSave="340" documentId="13_ncr:1_{4E4E044E-0397-49A1-8B73-67D9B76A8147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{864A7A3D-9D3D-4576-86ED-60270B1C440E}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12649" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Visual Object Recognition in the SelfStorage Business</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Das geplante Ergebnis ist eine benutzerfreundliche Darstellung mithilfe von React, welches das Datenmanagement im Programm ermöglicht.</t>
+  </si>
+  <si>
+    <t>Objekterkennung</t>
+  </si>
+  <si>
+    <t>Präsentation1</t>
   </si>
 </sst>
 </file>
@@ -289,7 +295,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,12 +316,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -323,6 +323,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE629"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -635,13 +653,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -652,36 +664,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -690,6 +719,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFE629"/>
+      <color rgb="FF00CC66"/>
       <color rgb="FF928100"/>
       <color rgb="FF33CCFF"/>
       <color rgb="FF685C00"/>
@@ -697,7 +728,6 @@
       <color rgb="FF009A00"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF00CC99"/>
-      <color rgb="FF00CC66"/>
     </mruColors>
   </colors>
   <extLst>
@@ -715,16 +745,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>31350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>700170</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>17094</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>700169</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>17093</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -933,16 +963,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>768061</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>62702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>41566</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>172580</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>172581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -994,15 +1024,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>209006</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>53120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>553865</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>175817</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1055,16 +1085,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>606117</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2469</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>595666</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>117422</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>167205</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>142124</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>156752</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>68972</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1094,7 +1124,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7127096" y="378679"/>
+          <a:off x="10377133" y="1434158"/>
           <a:ext cx="2821576" cy="1080181"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1116,15 +1146,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>119358</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>10448</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>653141</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>653143</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>90913</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1177,16 +1207,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>94052</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>62701</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>664155</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25078</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25079</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1238,15 +1268,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>553865</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>7248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>229907</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>25081</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1395,16 +1425,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>323959</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>547682</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>31350</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>31351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1456,16 +1486,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>282158</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>20901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>529550</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>75242</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>529551</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>75241</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1497,6 +1527,262 @@
         <a:xfrm>
           <a:off x="5172892" y="585217"/>
           <a:ext cx="1877637" cy="1935392"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="307238" cy="312463"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 8" descr="C# - Programmiersprache Logo Microsoft Visual Studio .NET Framework -  javascript Symbol png herunterladen - 800*800 - Kostenlos transparent C png  Herunterladen.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE87D68C-8F90-4CE6-A2C2-40D69ABBDAFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13041957" y="1692946"/>
+          <a:ext cx="307238" cy="312463"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="307238" cy="312464"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 9" descr="C# - Programmiersprache Logo Microsoft Visual Studio .NET Framework -  javascript Symbol png herunterladen - 800*800 - Kostenlos transparent C png  Herunterladen.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEDD8600-789C-4402-94AC-7484A20D8044}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13857079" y="752420"/>
+          <a:ext cx="307238" cy="312464"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="de-AT"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="307238" cy="312463"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 22" descr="Figma Vector Logo - Download Free SVG Icon | Worldvectorlogo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249018E0-6F2D-4390-B206-103387B44966}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13857079" y="1692946"/>
+          <a:ext cx="307238" cy="312463"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>809938</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>156755</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>797427</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>31350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Grafik 14" descr="Ubiquiti AI Theta - Discreet, Intelligent Surveillance | Scoop">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2CA81CF-6925-D69D-F435-561540FE2BD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15482139" y="1473491"/>
+          <a:ext cx="2432857" cy="1567542"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>106595</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>94053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>752420</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>39040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Grafik 15" descr="GitHub - ultralytics/yolov5: YOLOv5 🚀 in PyTorch &gt; ONNX &gt; CoreML &gt; TFLite">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD9A6451-D21B-0E1B-1916-2F66B3D5804D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="12231" t="29496" r="11510" b="18009"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15593918" y="3291840"/>
+          <a:ext cx="2276071" cy="1073619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1787,13 +2073,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH241"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="45.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.59765625" customWidth="1"/>
     <col min="3" max="3" width="10.69921875" style="9" customWidth="1"/>
     <col min="4" max="4" width="10.69921875" style="8" customWidth="1"/>
     <col min="5" max="33" width="3.59765625" customWidth="1"/>
@@ -1807,56 +2093,56 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="38" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="38" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="38" t="s">
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="38" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="38" t="s">
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="38" t="s">
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="38" t="s">
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="AH1" s="40"/>
+      <c r="AH1" s="32"/>
     </row>
     <row r="2" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
@@ -1969,7 +2255,8 @@
       <c r="D3" s="8">
         <v>2</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="47"/>
+      <c r="L3" s="51"/>
       <c r="AH3" s="14"/>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.3">
@@ -1982,7 +2269,8 @@
       <c r="D4" s="8">
         <v>5</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="47"/>
+      <c r="L4" s="14"/>
       <c r="AB4" t="s">
         <v>38</v>
       </c>
@@ -1998,9 +2286,10 @@
       <c r="D5" s="8">
         <v>4</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="37"/>
+      <c r="F5" s="47"/>
+      <c r="L5" s="14"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
       <c r="AH5" s="14"/>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.3">
@@ -2013,29 +2302,30 @@
       <c r="D6" s="8">
         <v>4</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="47"/>
+      <c r="L6" s="14"/>
       <c r="AH6" s="14"/>
     </row>
     <row r="7" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="49">
         <f>SUM(C3:C6)</f>
         <v>15</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="50">
         <f>SUM(D3:D6)</f>
         <v>15</v>
       </c>
       <c r="E7" s="23"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
+      <c r="L7" s="24"/>
       <c r="M7" s="23"/>
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
@@ -2069,7 +2359,8 @@
       <c r="D8" s="8">
         <v>5</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="47"/>
+      <c r="L8" s="14"/>
       <c r="AH8" s="14"/>
     </row>
     <row r="9" spans="2:34" x14ac:dyDescent="0.3">
@@ -2082,29 +2373,30 @@
       <c r="D9" s="8">
         <v>5</v>
       </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="47"/>
+      <c r="L9" s="14"/>
       <c r="AH9" s="14"/>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="49">
         <f>SUM(C8:C9)</f>
         <v>10</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="50">
         <f>SUM(D8:D9)</f>
         <v>10</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
       <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
+      <c r="L10" s="24"/>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
@@ -2135,8 +2427,9 @@
       <c r="C11" s="9">
         <v>15</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="L11" s="14"/>
       <c r="AH11" s="14"/>
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.3">
@@ -2146,8 +2439,9 @@
       <c r="C12" s="9">
         <v>20</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="14"/>
       <c r="AH12" s="14"/>
     </row>
     <row r="13" spans="2:34" x14ac:dyDescent="0.3">
@@ -2157,10 +2451,11 @@
       <c r="D13" s="8">
         <v>30</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="14"/>
       <c r="AH13" s="14"/>
     </row>
     <row r="14" spans="2:34" x14ac:dyDescent="0.3">
@@ -2173,7 +2468,7 @@
       <c r="D14" s="8">
         <v>10</v>
       </c>
-      <c r="L14" s="13"/>
+      <c r="L14" s="53"/>
       <c r="M14" s="13"/>
       <c r="AH14" s="14"/>
     </row>
@@ -2187,6 +2482,7 @@
       <c r="D15" s="8">
         <v>5</v>
       </c>
+      <c r="L15" s="14"/>
       <c r="N15" s="11"/>
       <c r="O15" s="13"/>
       <c r="AH15" s="14"/>
@@ -2198,6 +2494,7 @@
       <c r="D16" s="8">
         <v>20</v>
       </c>
+      <c r="L16" s="14"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
@@ -2213,8 +2510,9 @@
       <c r="D17" s="8">
         <v>25</v>
       </c>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
+      <c r="L17" s="14"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
       <c r="R17" s="13"/>
       <c r="S17" s="13"/>
       <c r="T17" s="13"/>
@@ -2239,7 +2537,7 @@
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
+      <c r="L18" s="24"/>
       <c r="M18" s="23"/>
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
@@ -2273,6 +2571,7 @@
       <c r="D19" s="8">
         <v>10</v>
       </c>
+      <c r="L19" s="14"/>
       <c r="V19" s="13"/>
       <c r="AH19" s="14"/>
     </row>
@@ -2286,6 +2585,7 @@
       <c r="D20" s="8">
         <v>10</v>
       </c>
+      <c r="L20" s="14"/>
       <c r="W20" s="13"/>
       <c r="AH20" s="14"/>
     </row>
@@ -2299,6 +2599,7 @@
       <c r="D21" s="8">
         <v>8</v>
       </c>
+      <c r="L21" s="14"/>
       <c r="X21" s="13"/>
       <c r="AH21" s="14"/>
     </row>
@@ -2312,6 +2613,7 @@
       <c r="D22" s="8">
         <v>5</v>
       </c>
+      <c r="L22" s="14"/>
       <c r="Y22" s="13"/>
       <c r="AH22" s="14"/>
     </row>
@@ -2334,7 +2636,7 @@
       <c r="I23" s="23"/>
       <c r="J23" s="23"/>
       <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
+      <c r="L23" s="24"/>
       <c r="M23" s="23"/>
       <c r="N23" s="23"/>
       <c r="O23" s="23"/>
@@ -2368,6 +2670,7 @@
       <c r="D24" s="8">
         <v>30</v>
       </c>
+      <c r="L24" s="14"/>
       <c r="AA24" s="13"/>
       <c r="AB24" s="13"/>
       <c r="AC24" s="13"/>
@@ -2384,6 +2687,7 @@
       <c r="D25" s="8">
         <v>5</v>
       </c>
+      <c r="L25" s="14"/>
       <c r="AE25" s="13"/>
       <c r="AH25" s="14"/>
     </row>
@@ -2406,7 +2710,7 @@
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
+      <c r="L26" s="24"/>
       <c r="M26" s="23"/>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -2449,7 +2753,7 @@
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
+      <c r="L27" s="19"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
       <c r="O27" s="18"/>
@@ -2475,6 +2779,9 @@
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.3">
       <c r="D28" s="9"/>
+      <c r="K28" t="s">
+        <v>61</v>
+      </c>
       <c r="AH28"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.3">
@@ -3331,16 +3638,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="T1:X1"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3351,8 +3658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CAAB76-81FF-479D-9151-CB58DF96AA0A}">
   <dimension ref="A1:AG110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3366,1759 +3673,1768 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-    </row>
-    <row r="2" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
       <c r="J3" s="26"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="32"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="32"/>
-      <c r="AD3" s="32"/>
-      <c r="AE3" s="32"/>
-      <c r="AF3" s="32"/>
-      <c r="AG3" s="32"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="26"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="26"/>
+      <c r="AE3" s="26"/>
+      <c r="AF3" s="26"/>
+      <c r="AG3" s="26"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="26"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="32"/>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="32"/>
-      <c r="AF4" s="32"/>
-      <c r="AG4" s="32"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="26"/>
+    </row>
+    <row r="5" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
       <c r="J5" s="26"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="32"/>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="32"/>
-      <c r="AF5" s="32"/>
-      <c r="AG5" s="32"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="32"/>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="32"/>
-      <c r="AE6" s="32"/>
-      <c r="AF6" s="32"/>
-      <c r="AG6" s="32"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="E6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="36"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="36"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="36"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="U6" s="36"/>
+      <c r="V6" s="39"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+      <c r="AG6" s="26"/>
+    </row>
+    <row r="7" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="32"/>
-      <c r="AA7" s="32"/>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="32"/>
-      <c r="AD7" s="32"/>
-      <c r="AE7" s="32"/>
-      <c r="AF7" s="32"/>
-      <c r="AG7" s="32"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="26"/>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="26"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="32"/>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="32"/>
-      <c r="AC8" s="32"/>
-      <c r="AD8" s="32"/>
-      <c r="AE8" s="32"/>
-      <c r="AF8" s="32"/>
-      <c r="AG8" s="32"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="42"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="26"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="32"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="32"/>
-      <c r="AA9" s="32"/>
-      <c r="AB9" s="32"/>
-      <c r="AC9" s="32"/>
-      <c r="AD9" s="32"/>
-      <c r="AE9" s="32"/>
-      <c r="AF9" s="32"/>
-      <c r="AG9" s="32"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="32"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="32"/>
-      <c r="AC10" s="32"/>
-      <c r="AD10" s="32"/>
-      <c r="AE10" s="32"/>
-      <c r="AF10" s="32"/>
-      <c r="AG10" s="32"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
+      <c r="AA10" s="26"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="26"/>
+      <c r="AG10" s="26"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="32"/>
-      <c r="AA11" s="32"/>
-      <c r="AB11" s="32"/>
-      <c r="AC11" s="32"/>
-      <c r="AD11" s="32"/>
-      <c r="AE11" s="32"/>
-      <c r="AF11" s="32"/>
-      <c r="AG11" s="32"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="26"/>
+      <c r="AD11" s="26"/>
+      <c r="AE11" s="26"/>
+      <c r="AF11" s="26"/>
+      <c r="AG11" s="26"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="32"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="32"/>
-      <c r="AC12" s="32"/>
-      <c r="AD12" s="32"/>
-      <c r="AE12" s="32"/>
-      <c r="AF12" s="32"/>
-      <c r="AG12" s="32"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="26"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="32"/>
-      <c r="AC13" s="32"/>
-      <c r="AD13" s="32"/>
-      <c r="AE13" s="32"/>
-      <c r="AF13" s="32"/>
-      <c r="AG13" s="32"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+      <c r="AC13" s="26"/>
+      <c r="AD13" s="26"/>
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="26"/>
+      <c r="AG13" s="26"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="32"/>
-      <c r="AC14" s="32"/>
-      <c r="AD14" s="32"/>
-      <c r="AE14" s="32"/>
-      <c r="AF14" s="32"/>
-      <c r="AG14" s="32"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
+      <c r="AC14" s="26"/>
+      <c r="AD14" s="26"/>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="32"/>
-      <c r="AA15" s="32"/>
-      <c r="AB15" s="32"/>
-      <c r="AC15" s="32"/>
-      <c r="AD15" s="32"/>
-      <c r="AE15" s="32"/>
-      <c r="AF15" s="32"/>
-      <c r="AG15" s="32"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="26"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="32"/>
-      <c r="X16" s="32"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="32"/>
-      <c r="AC16" s="32"/>
-      <c r="AD16" s="32"/>
-      <c r="AE16" s="32"/>
-      <c r="AF16" s="32"/>
-      <c r="AG16" s="32"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="26"/>
+      <c r="AA16" s="26"/>
+      <c r="AB16" s="26"/>
+      <c r="AC16" s="26"/>
+      <c r="AD16" s="26"/>
+      <c r="AE16" s="26"/>
+      <c r="AF16" s="26"/>
+      <c r="AG16" s="26"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="32"/>
-      <c r="AC17" s="32"/>
-      <c r="AD17" s="32"/>
-      <c r="AE17" s="32"/>
-      <c r="AF17" s="32"/>
-      <c r="AG17" s="32"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="26"/>
+      <c r="AB17" s="26"/>
+      <c r="AC17" s="26"/>
+      <c r="AD17" s="26"/>
+      <c r="AE17" s="26"/>
+      <c r="AF17" s="26"/>
+      <c r="AG17" s="26"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="32"/>
-      <c r="AC18" s="32"/>
-      <c r="AD18" s="32"/>
-      <c r="AE18" s="32"/>
-      <c r="AF18" s="32"/>
-      <c r="AG18" s="32"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="43"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
+      <c r="AC18" s="26"/>
+      <c r="AD18" s="26"/>
+      <c r="AE18" s="26"/>
+      <c r="AF18" s="26"/>
+      <c r="AG18" s="26"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="32"/>
-      <c r="W19" s="32"/>
-      <c r="X19" s="32"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="32"/>
-      <c r="AA19" s="32"/>
-      <c r="AB19" s="32"/>
-      <c r="AC19" s="32"/>
-      <c r="AD19" s="32"/>
-      <c r="AE19" s="32"/>
-      <c r="AF19" s="32"/>
-      <c r="AG19" s="32"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="43"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="26"/>
+      <c r="AD19" s="26"/>
+      <c r="AE19" s="26"/>
+      <c r="AF19" s="26"/>
+      <c r="AG19" s="26"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="32"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="32"/>
-      <c r="AB20" s="32"/>
-      <c r="AC20" s="32"/>
-      <c r="AD20" s="32"/>
-      <c r="AE20" s="32"/>
-      <c r="AF20" s="32"/>
-      <c r="AG20" s="32"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="26"/>
+      <c r="AD20" s="26"/>
+      <c r="AE20" s="26"/>
+      <c r="AF20" s="26"/>
+      <c r="AG20" s="26"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="32"/>
-      <c r="W21" s="32"/>
-      <c r="X21" s="32"/>
-      <c r="Y21" s="32"/>
-      <c r="Z21" s="32"/>
-      <c r="AA21" s="32"/>
-      <c r="AB21" s="32"/>
-      <c r="AC21" s="32"/>
-      <c r="AD21" s="32"/>
-      <c r="AE21" s="32"/>
-      <c r="AF21" s="32"/>
-      <c r="AG21" s="32"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
+      <c r="AC21" s="26"/>
+      <c r="AD21" s="26"/>
+      <c r="AE21" s="26"/>
+      <c r="AF21" s="26"/>
+      <c r="AG21" s="26"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
-      <c r="V22" s="32"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32"/>
-      <c r="AA22" s="32"/>
-      <c r="AB22" s="32"/>
-      <c r="AC22" s="32"/>
-      <c r="AD22" s="32"/>
-      <c r="AE22" s="32"/>
-      <c r="AF22" s="32"/>
-      <c r="AG22" s="32"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="26"/>
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="26"/>
+      <c r="AF22" s="26"/>
+      <c r="AG22" s="26"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="32"/>
-      <c r="S23" s="32"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="32"/>
-      <c r="V23" s="32"/>
-      <c r="W23" s="32"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="32"/>
-      <c r="AA23" s="32"/>
-      <c r="AB23" s="32"/>
-      <c r="AC23" s="32"/>
-      <c r="AD23" s="32"/>
-      <c r="AE23" s="32"/>
-      <c r="AF23" s="32"/>
-      <c r="AG23" s="32"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="42"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="42"/>
+      <c r="U23" s="42"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="26"/>
+      <c r="AD23" s="26"/>
+      <c r="AE23" s="26"/>
+      <c r="AF23" s="26"/>
+      <c r="AG23" s="26"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="32"/>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="32"/>
-      <c r="AC24" s="32"/>
-      <c r="AD24" s="32"/>
-      <c r="AE24" s="32"/>
-      <c r="AF24" s="32"/>
-      <c r="AG24" s="32"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="42"/>
+      <c r="V24" s="43"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26"/>
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="26"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="32"/>
-      <c r="S25" s="32"/>
-      <c r="T25" s="32"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="32"/>
-      <c r="W25" s="32"/>
-      <c r="X25" s="32"/>
-      <c r="Y25" s="32"/>
-      <c r="Z25" s="32"/>
-      <c r="AA25" s="32"/>
-      <c r="AB25" s="32"/>
-      <c r="AC25" s="32"/>
-      <c r="AD25" s="32"/>
-      <c r="AE25" s="32"/>
-      <c r="AF25" s="32"/>
-      <c r="AG25" s="32"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="43"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="26"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="26"/>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="26"/>
+      <c r="AD25" s="26"/>
+      <c r="AE25" s="26"/>
+      <c r="AF25" s="26"/>
+      <c r="AG25" s="26"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="32"/>
-      <c r="S26" s="32"/>
-      <c r="T26" s="32"/>
-      <c r="U26" s="32"/>
-      <c r="V26" s="32"/>
-      <c r="W26" s="32"/>
-      <c r="X26" s="32"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="32"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="32"/>
-      <c r="AC26" s="32"/>
-      <c r="AD26" s="32"/>
-      <c r="AE26" s="32"/>
-      <c r="AF26" s="32"/>
-      <c r="AG26" s="32"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="43"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="26"/>
+      <c r="AC26" s="26"/>
+      <c r="AD26" s="26"/>
+      <c r="AE26" s="26"/>
+      <c r="AF26" s="26"/>
+      <c r="AG26" s="26"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="26"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="32"/>
-      <c r="R27" s="32"/>
-      <c r="S27" s="32"/>
-      <c r="T27" s="32"/>
-      <c r="U27" s="32"/>
-      <c r="V27" s="32"/>
-      <c r="W27" s="32"/>
-      <c r="X27" s="32"/>
-      <c r="Y27" s="32"/>
-      <c r="Z27" s="32"/>
-      <c r="AA27" s="32"/>
-      <c r="AB27" s="32"/>
-      <c r="AC27" s="32"/>
-      <c r="AD27" s="32"/>
-      <c r="AE27" s="32"/>
-      <c r="AF27" s="32"/>
-      <c r="AG27" s="32"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+      <c r="Y27" s="26"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="26"/>
+      <c r="AC27" s="26"/>
+      <c r="AD27" s="26"/>
+      <c r="AE27" s="26"/>
+      <c r="AF27" s="26"/>
+      <c r="AG27" s="26"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="32"/>
-      <c r="R28" s="32"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="32"/>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="32"/>
-      <c r="X28" s="32"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="32"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="32"/>
-      <c r="AC28" s="32"/>
-      <c r="AD28" s="32"/>
-      <c r="AE28" s="32"/>
-      <c r="AF28" s="32"/>
-      <c r="AG28" s="32"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="42"/>
+      <c r="V28" s="43"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="26"/>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="26"/>
+      <c r="AE28" s="26"/>
+      <c r="AF28" s="26"/>
+      <c r="AG28" s="26"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="32"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="32"/>
-      <c r="U29" s="32"/>
-      <c r="V29" s="32"/>
-      <c r="W29" s="32"/>
-      <c r="X29" s="32"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="32"/>
-      <c r="AD29" s="32"/>
-      <c r="AE29" s="32"/>
-      <c r="AF29" s="32"/>
-      <c r="AG29" s="32"/>
-    </row>
-    <row r="30" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="32"/>
-      <c r="R30" s="32"/>
-      <c r="S30" s="32"/>
-      <c r="T30" s="32"/>
-      <c r="U30" s="32"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="32"/>
-      <c r="X30" s="32"/>
-      <c r="Y30" s="32"/>
-      <c r="Z30" s="32"/>
-      <c r="AA30" s="32"/>
-      <c r="AB30" s="32"/>
-      <c r="AC30" s="32"/>
-      <c r="AD30" s="32"/>
-      <c r="AE30" s="32"/>
-      <c r="AF30" s="32"/>
-      <c r="AG30" s="32"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="42"/>
+      <c r="U29" s="42"/>
+      <c r="V29" s="43"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="26"/>
+      <c r="AC29" s="26"/>
+      <c r="AD29" s="26"/>
+      <c r="AE29" s="26"/>
+      <c r="AF29" s="26"/>
+      <c r="AG29" s="26"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="42"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="42"/>
+      <c r="U30" s="42"/>
+      <c r="V30" s="43"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="26"/>
+      <c r="AD30" s="26"/>
+      <c r="AE30" s="26"/>
+      <c r="AF30" s="26"/>
+      <c r="AG30" s="26"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="32"/>
-      <c r="R31" s="32"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="32"/>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="32"/>
-      <c r="X31" s="32"/>
-      <c r="Y31" s="32"/>
-      <c r="Z31" s="32"/>
-      <c r="AA31" s="32"/>
-      <c r="AB31" s="32"/>
-      <c r="AC31" s="32"/>
-      <c r="AD31" s="32"/>
-      <c r="AE31" s="32"/>
-      <c r="AF31" s="32"/>
-      <c r="AG31" s="32"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="42"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="42"/>
+      <c r="V31" s="43"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+      <c r="Y31" s="26"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="26"/>
+      <c r="AB31" s="26"/>
+      <c r="AC31" s="26"/>
+      <c r="AD31" s="26"/>
+      <c r="AE31" s="26"/>
+      <c r="AF31" s="26"/>
+      <c r="AG31" s="26"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="32"/>
-      <c r="S32" s="32"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="32"/>
-      <c r="X32" s="32"/>
-      <c r="Y32" s="32"/>
-      <c r="Z32" s="32"/>
-      <c r="AA32" s="32"/>
-      <c r="AB32" s="32"/>
-      <c r="AC32" s="32"/>
-      <c r="AD32" s="32"/>
-      <c r="AE32" s="32"/>
-      <c r="AF32" s="32"/>
-      <c r="AG32" s="32"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="42"/>
+      <c r="U32" s="42"/>
+      <c r="V32" s="43"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="26"/>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="26"/>
+      <c r="AF32" s="26"/>
+      <c r="AG32" s="26"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
-      <c r="R33" s="32"/>
-      <c r="S33" s="32"/>
-      <c r="T33" s="32"/>
-      <c r="U33" s="32"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="32"/>
-      <c r="X33" s="32"/>
-      <c r="Y33" s="32"/>
-      <c r="Z33" s="32"/>
-      <c r="AA33" s="32"/>
-      <c r="AB33" s="32"/>
-      <c r="AC33" s="32"/>
-      <c r="AD33" s="32"/>
-      <c r="AE33" s="32"/>
-      <c r="AF33" s="32"/>
-      <c r="AG33" s="32"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="42"/>
+      <c r="U33" s="42"/>
+      <c r="V33" s="43"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="26"/>
+      <c r="AC33" s="26"/>
+      <c r="AD33" s="26"/>
+      <c r="AE33" s="26"/>
+      <c r="AF33" s="26"/>
+      <c r="AG33" s="26"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="32"/>
-      <c r="R34" s="32"/>
-      <c r="S34" s="32"/>
-      <c r="T34" s="32"/>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
-      <c r="W34" s="32"/>
-      <c r="X34" s="32"/>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="32"/>
-      <c r="R35" s="32"/>
-      <c r="S35" s="32"/>
-      <c r="T35" s="32"/>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
-      <c r="W35" s="32"/>
-      <c r="X35" s="32"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="42"/>
+      <c r="S34" s="43"/>
+      <c r="T34" s="42"/>
+      <c r="U34" s="42"/>
+      <c r="V34" s="43"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+    </row>
+    <row r="35" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="45"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="46"/>
+      <c r="T35" s="45"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="26"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="32"/>
-      <c r="R36" s="32"/>
-      <c r="S36" s="32"/>
-      <c r="T36" s="32"/>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="32"/>
-      <c r="X36" s="32"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="26"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="32"/>
-      <c r="R37" s="32"/>
-      <c r="S37" s="32"/>
-      <c r="T37" s="32"/>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
-      <c r="W37" s="32"/>
-      <c r="X37" s="32"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="32"/>
-      <c r="S38" s="32"/>
-      <c r="T38" s="32"/>
-      <c r="U38" s="32"/>
-      <c r="V38" s="32"/>
-      <c r="W38" s="32"/>
-      <c r="X38" s="32"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A39" s="32"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32"/>
-      <c r="R39" s="32"/>
-      <c r="S39" s="32"/>
-      <c r="T39" s="32"/>
-      <c r="U39" s="32"/>
-      <c r="V39" s="32"/>
-      <c r="W39" s="32"/>
-      <c r="X39" s="32"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A40" s="32"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="32"/>
-      <c r="R40" s="32"/>
-      <c r="S40" s="32"/>
-      <c r="T40" s="32"/>
-      <c r="U40" s="32"/>
-      <c r="V40" s="32"/>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A41" s="32"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="S41" s="32"/>
-      <c r="T41" s="32"/>
-      <c r="U41" s="32"/>
-      <c r="V41" s="32"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="32"/>
-      <c r="R42" s="32"/>
-      <c r="S42" s="32"/>
-      <c r="T42" s="32"/>
-      <c r="U42" s="32"/>
-      <c r="V42" s="32"/>
-      <c r="W42" s="32"/>
-      <c r="X42" s="32"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="26"/>
+      <c r="T42" s="26"/>
+      <c r="U42" s="26"/>
+      <c r="V42" s="26"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A43" s="32"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="32"/>
-      <c r="R43" s="32"/>
-      <c r="S43" s="32"/>
-      <c r="T43" s="32"/>
-      <c r="U43" s="32"/>
-      <c r="V43" s="32"/>
-      <c r="W43" s="32"/>
-      <c r="X43" s="32"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="26"/>
+      <c r="T43" s="26"/>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
-      <c r="O44" s="32"/>
-      <c r="P44" s="32"/>
-      <c r="Q44" s="32"/>
-      <c r="R44" s="32"/>
-      <c r="S44" s="32"/>
-      <c r="T44" s="32"/>
-      <c r="U44" s="32"/>
-      <c r="V44" s="32"/>
-      <c r="W44" s="32"/>
-      <c r="X44" s="32"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="26"/>
+      <c r="T44" s="26"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="32"/>
-      <c r="R45" s="32"/>
-      <c r="S45" s="32"/>
-      <c r="T45" s="32"/>
-      <c r="U45" s="32"/>
-      <c r="V45" s="32"/>
-      <c r="W45" s="32"/>
-      <c r="X45" s="32"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="26"/>
+      <c r="T45" s="26"/>
+      <c r="U45" s="26"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="32"/>
-      <c r="R46" s="32"/>
-      <c r="S46" s="32"/>
-      <c r="T46" s="32"/>
-      <c r="U46" s="32"/>
-      <c r="V46" s="32"/>
-      <c r="W46" s="32"/>
-      <c r="X46" s="32"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
+      <c r="P46" s="26"/>
+      <c r="Q46" s="26"/>
+      <c r="R46" s="26"/>
+      <c r="S46" s="26"/>
+      <c r="T46" s="26"/>
+      <c r="U46" s="26"/>
+      <c r="V46" s="26"/>
+      <c r="W46" s="26"/>
+      <c r="X46" s="26"/>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="32"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="32"/>
-      <c r="V47" s="32"/>
-      <c r="W47" s="32"/>
-      <c r="X47" s="32"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="26"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="26"/>
+      <c r="T47" s="26"/>
+      <c r="U47" s="26"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="26"/>
+      <c r="X47" s="26"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="32"/>
-      <c r="R48" s="32"/>
-      <c r="S48" s="32"/>
-      <c r="T48" s="32"/>
-      <c r="U48" s="32"/>
-      <c r="V48" s="32"/>
-      <c r="W48" s="32"/>
-      <c r="X48" s="32"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="26"/>
+      <c r="R48" s="26"/>
+      <c r="S48" s="26"/>
+      <c r="T48" s="26"/>
+      <c r="U48" s="26"/>
+      <c r="V48" s="26"/>
+      <c r="W48" s="26"/>
+      <c r="X48" s="26"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="32"/>
-      <c r="R49" s="32"/>
-      <c r="S49" s="32"/>
-      <c r="T49" s="32"/>
-      <c r="U49" s="32"/>
-      <c r="V49" s="32"/>
-      <c r="W49" s="32"/>
-      <c r="X49" s="32"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="26"/>
+      <c r="R49" s="26"/>
+      <c r="S49" s="26"/>
+      <c r="T49" s="26"/>
+      <c r="U49" s="26"/>
+      <c r="V49" s="26"/>
+      <c r="W49" s="26"/>
+      <c r="X49" s="26"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="32"/>
-      <c r="N50" s="32"/>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="32"/>
-      <c r="R50" s="32"/>
-      <c r="S50" s="32"/>
-      <c r="T50" s="32"/>
-      <c r="U50" s="32"/>
-      <c r="V50" s="32"/>
-      <c r="W50" s="32"/>
-      <c r="X50" s="32"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
+      <c r="P50" s="26"/>
+      <c r="Q50" s="26"/>
+      <c r="R50" s="26"/>
+      <c r="S50" s="26"/>
+      <c r="T50" s="26"/>
+      <c r="U50" s="26"/>
+      <c r="V50" s="26"/>
+      <c r="W50" s="26"/>
+      <c r="X50" s="26"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A51" s="32"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="32"/>
-      <c r="R51" s="32"/>
-      <c r="S51" s="32"/>
-      <c r="T51" s="32"/>
-      <c r="U51" s="32"/>
-      <c r="V51" s="32"/>
-      <c r="W51" s="32"/>
-      <c r="X51" s="32"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="26"/>
+      <c r="Q51" s="26"/>
+      <c r="R51" s="26"/>
+      <c r="S51" s="26"/>
+      <c r="T51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="V51" s="26"/>
+      <c r="W51" s="26"/>
+      <c r="X51" s="26"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
-      <c r="O52" s="32"/>
-      <c r="P52" s="32"/>
-      <c r="Q52" s="32"/>
-      <c r="R52" s="32"/>
-      <c r="S52" s="32"/>
-      <c r="T52" s="32"/>
-      <c r="U52" s="32"/>
-      <c r="V52" s="32"/>
-      <c r="W52" s="32"/>
-      <c r="X52" s="32"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="26"/>
+      <c r="Q52" s="26"/>
+      <c r="R52" s="26"/>
+      <c r="S52" s="26"/>
+      <c r="T52" s="26"/>
+      <c r="U52" s="26"/>
+      <c r="V52" s="26"/>
+      <c r="W52" s="26"/>
+      <c r="X52" s="26"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A53" s="32"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-      <c r="M53" s="32"/>
-      <c r="N53" s="32"/>
-      <c r="O53" s="32"/>
-      <c r="P53" s="32"/>
-      <c r="Q53" s="32"/>
-      <c r="R53" s="32"/>
-      <c r="S53" s="32"/>
-      <c r="T53" s="32"/>
-      <c r="U53" s="32"/>
-      <c r="V53" s="32"/>
-      <c r="W53" s="32"/>
-      <c r="X53" s="32"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
+      <c r="P53" s="26"/>
+      <c r="Q53" s="26"/>
+      <c r="R53" s="26"/>
+      <c r="S53" s="26"/>
+      <c r="T53" s="26"/>
+      <c r="U53" s="26"/>
+      <c r="V53" s="26"/>
+      <c r="W53" s="26"/>
+      <c r="X53" s="26"/>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="32"/>
-      <c r="N54" s="32"/>
-      <c r="O54" s="32"/>
-      <c r="P54" s="32"/>
-      <c r="Q54" s="32"/>
-      <c r="R54" s="32"/>
-      <c r="S54" s="32"/>
-      <c r="T54" s="32"/>
-      <c r="U54" s="32"/>
-      <c r="V54" s="32"/>
-      <c r="W54" s="32"/>
-      <c r="X54" s="32"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
+      <c r="Q54" s="26"/>
+      <c r="R54" s="26"/>
+      <c r="S54" s="26"/>
+      <c r="T54" s="26"/>
+      <c r="U54" s="26"/>
+      <c r="V54" s="26"/>
+      <c r="W54" s="26"/>
+      <c r="X54" s="26"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A55" s="32"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32"/>
-      <c r="Q55" s="32"/>
-      <c r="R55" s="32"/>
-      <c r="S55" s="32"/>
-      <c r="T55" s="32"/>
-      <c r="U55" s="32"/>
-      <c r="V55" s="32"/>
-      <c r="W55" s="32"/>
-      <c r="X55" s="32"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="26"/>
+      <c r="O55" s="26"/>
+      <c r="P55" s="26"/>
+      <c r="Q55" s="26"/>
+      <c r="R55" s="26"/>
+      <c r="S55" s="26"/>
+      <c r="T55" s="26"/>
+      <c r="U55" s="26"/>
+      <c r="V55" s="26"/>
+      <c r="W55" s="26"/>
+      <c r="X55" s="26"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A56" s="32"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="32"/>
-      <c r="O56" s="32"/>
-      <c r="P56" s="32"/>
-      <c r="Q56" s="32"/>
-      <c r="R56" s="32"/>
-      <c r="S56" s="32"/>
-      <c r="T56" s="32"/>
-      <c r="U56" s="32"/>
-      <c r="V56" s="32"/>
-      <c r="W56" s="32"/>
-      <c r="X56" s="32"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="26"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
+      <c r="P56" s="26"/>
+      <c r="Q56" s="26"/>
+      <c r="R56" s="26"/>
+      <c r="S56" s="26"/>
+      <c r="T56" s="26"/>
+      <c r="U56" s="26"/>
+      <c r="V56" s="26"/>
+      <c r="W56" s="26"/>
+      <c r="X56" s="26"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57"/>
@@ -5231,12 +5547,13 @@
     <row r="109" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="110" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="G1:I2"/>
-    <mergeCell ref="J1:L2"/>
-    <mergeCell ref="M1:O2"/>
+  <mergeCells count="6">
+    <mergeCell ref="T6:V7"/>
+    <mergeCell ref="E6:G7"/>
+    <mergeCell ref="H6:J7"/>
+    <mergeCell ref="K6:M7"/>
+    <mergeCell ref="N6:P7"/>
+    <mergeCell ref="Q6:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5255,88 +5572,88 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="27" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="30" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="30" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="30" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H17" s="34" t="s">
+      <c r="H17" s="28" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="29" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5350,7 +5667,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Start Doku + Regristrierungsfehler Behoben
</commit_message>
<xml_diff>
--- a/Dokumente/20240913_Zeitplan.xlsx
+++ b/Dokumente/20240913_Zeitplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c9cb578a977eee7/Desktop/project/diplomarbeit/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\diplomarbeit\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="340" documentId="13_ncr:1_{4E4E044E-0397-49A1-8B73-67D9B76A8147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{864A7A3D-9D3D-4576-86ED-60270B1C440E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224C37A4-F178-4E34-A7A8-03561F7DE9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="29699" windowHeight="16796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Visual Object Recognition in the SelfStorage Business</t>
   </si>
@@ -247,12 +247,15 @@
   <si>
     <t>Präsentation1</t>
   </si>
+  <si>
+    <t>Präsentation 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +296,37 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -340,12 +374,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE629"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -594,11 +628,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -664,36 +740,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -709,8 +755,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -719,13 +810,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF009A00"/>
+      <color rgb="FF00CC66"/>
       <color rgb="FFFFE629"/>
-      <color rgb="FF00CC66"/>
       <color rgb="FF928100"/>
       <color rgb="FF33CCFF"/>
       <color rgb="FF685C00"/>
       <color rgb="FFFDE100"/>
-      <color rgb="FF009A00"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF00CC99"/>
     </mruColors>
@@ -1484,67 +1575,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>282158</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>20901</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>529551</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>75241</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2" descr="Mongodb plain Wortmarke logo - Soziale Medien und Logos Symbole">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D61F46C-E668-9D49-9EA2-1AADE52A6B1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5172892" y="585217"/>
-          <a:ext cx="1877637" cy="1935392"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
@@ -1708,7 +1738,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1769,7 +1799,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1801,11 +1831,129 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>146305</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>169569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>540573</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>2091</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F5F629C-65EC-A0D8-D2ED-4621BD2B76B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8297528" y="1486305"/>
+          <a:ext cx="2024512" cy="2089783"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>52252</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>67109</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>762870</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>36578</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Grafik 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA26D888-8F78-1E77-0199-EB9E4EE93069}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15539575" y="4205422"/>
+          <a:ext cx="2340864" cy="2414836"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2071,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AH241"/>
+  <dimension ref="A1:AS241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2089,62 +2237,75 @@
     <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="26"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33" t="s">
+      <c r="F1" s="45"/>
+      <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="33" t="s">
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="33" t="s">
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="33" t="s">
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="33" t="s">
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="33" t="s">
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="AH1" s="32"/>
-    </row>
-    <row r="2" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+    </row>
+    <row r="2" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="26"/>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2199,7 +2360,7 @@
       <c r="S2" s="6">
         <v>52</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="54">
         <v>1</v>
       </c>
       <c r="U2" s="6">
@@ -2244,8 +2405,20 @@
       <c r="AH2" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+      <c r="AP2" s="26"/>
+      <c r="AQ2" s="26"/>
+      <c r="AR2" s="26"/>
+      <c r="AS2" s="26"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
@@ -2255,11 +2428,24 @@
       <c r="D3" s="8">
         <v>2</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="L3" s="51"/>
+      <c r="E3" s="37"/>
+      <c r="L3" s="41"/>
+      <c r="T3" s="55"/>
       <c r="AH3" s="14"/>
-    </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI3" s="26"/>
+      <c r="AJ3" s="26"/>
+      <c r="AK3" s="26"/>
+      <c r="AL3" s="26"/>
+      <c r="AM3" s="26"/>
+      <c r="AN3" s="26"/>
+      <c r="AO3" s="26"/>
+      <c r="AP3" s="26"/>
+      <c r="AQ3" s="26"/>
+      <c r="AR3" s="26"/>
+      <c r="AS3" s="26"/>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
       <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
@@ -2269,14 +2455,27 @@
       <c r="D4" s="8">
         <v>5</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="37"/>
       <c r="L4" s="14"/>
-      <c r="AB4" t="s">
+      <c r="T4" s="56"/>
+      <c r="AB4" s="59" t="s">
         <v>38</v>
       </c>
       <c r="AH4" s="14"/>
-    </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="26"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="26"/>
+      <c r="AM4" s="26"/>
+      <c r="AN4" s="26"/>
+      <c r="AO4" s="26"/>
+      <c r="AP4" s="26"/>
+      <c r="AQ4" s="26"/>
+      <c r="AR4" s="26"/>
+      <c r="AS4" s="26"/>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
@@ -2286,13 +2485,26 @@
       <c r="D5" s="8">
         <v>4</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="37"/>
       <c r="L5" s="14"/>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
+      <c r="T5" s="56"/>
+      <c r="AB5" s="42"/>
+      <c r="AC5" s="42"/>
       <c r="AH5" s="14"/>
-    </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI5" s="26"/>
+      <c r="AJ5" s="26"/>
+      <c r="AK5" s="26"/>
+      <c r="AL5" s="26"/>
+      <c r="AM5" s="26"/>
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="26"/>
+      <c r="AP5" s="26"/>
+      <c r="AQ5" s="26"/>
+      <c r="AR5" s="26"/>
+      <c r="AS5" s="26"/>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
       <c r="B6" s="12" t="s">
         <v>30</v>
       </c>
@@ -2302,24 +2514,37 @@
       <c r="D6" s="8">
         <v>4</v>
       </c>
-      <c r="F6" s="47"/>
+      <c r="F6" s="37"/>
       <c r="L6" s="14"/>
+      <c r="T6" s="56"/>
       <c r="AH6" s="14"/>
-    </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="AI6" s="26"/>
+      <c r="AJ6" s="26"/>
+      <c r="AK6" s="26"/>
+      <c r="AL6" s="26"/>
+      <c r="AM6" s="26"/>
+      <c r="AN6" s="26"/>
+      <c r="AO6" s="26"/>
+      <c r="AP6" s="26"/>
+      <c r="AQ6" s="26"/>
+      <c r="AR6" s="26"/>
+      <c r="AS6" s="26"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="39">
         <f>SUM(C3:C6)</f>
         <v>15</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="40">
         <f>SUM(D3:D6)</f>
         <v>15</v>
       </c>
       <c r="E7" s="23"/>
-      <c r="F7" s="49"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
@@ -2333,7 +2558,7 @@
       <c r="Q7" s="23"/>
       <c r="R7" s="23"/>
       <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
+      <c r="T7" s="57"/>
       <c r="U7" s="23"/>
       <c r="V7" s="23"/>
       <c r="W7" s="23"/>
@@ -2348,8 +2573,20 @@
       <c r="AF7" s="23"/>
       <c r="AG7" s="23"/>
       <c r="AH7" s="24"/>
-    </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI7" s="26"/>
+      <c r="AJ7" s="26"/>
+      <c r="AK7" s="26"/>
+      <c r="AL7" s="26"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="26"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="26"/>
+      <c r="AQ7" s="26"/>
+      <c r="AR7" s="26"/>
+      <c r="AS7" s="26"/>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A8" s="26"/>
       <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
@@ -2359,11 +2596,24 @@
       <c r="D8" s="8">
         <v>5</v>
       </c>
-      <c r="G8" s="47"/>
+      <c r="G8" s="37"/>
       <c r="L8" s="14"/>
+      <c r="T8" s="56"/>
       <c r="AH8" s="14"/>
-    </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="26"/>
+      <c r="AM8" s="26"/>
+      <c r="AN8" s="26"/>
+      <c r="AO8" s="26"/>
+      <c r="AP8" s="26"/>
+      <c r="AQ8" s="26"/>
+      <c r="AR8" s="26"/>
+      <c r="AS8" s="26"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
       <c r="B9" s="12" t="s">
         <v>24</v>
       </c>
@@ -2373,25 +2623,38 @@
       <c r="D9" s="8">
         <v>5</v>
       </c>
-      <c r="G9" s="47"/>
+      <c r="G9" s="37"/>
       <c r="L9" s="14"/>
+      <c r="T9" s="56"/>
       <c r="AH9" s="14"/>
-    </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B10" s="48" t="s">
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26"/>
+      <c r="AM9" s="26"/>
+      <c r="AN9" s="26"/>
+      <c r="AO9" s="26"/>
+      <c r="AP9" s="26"/>
+      <c r="AQ9" s="26"/>
+      <c r="AR9" s="26"/>
+      <c r="AS9" s="26"/>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="39">
         <f>SUM(C8:C9)</f>
         <v>10</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="40">
         <f>SUM(D8:D9)</f>
         <v>10</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="49"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
@@ -2404,7 +2667,7 @@
       <c r="Q10" s="23"/>
       <c r="R10" s="23"/>
       <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
+      <c r="T10" s="57"/>
       <c r="U10" s="23"/>
       <c r="V10" s="23"/>
       <c r="W10" s="23"/>
@@ -2419,46 +2682,97 @@
       <c r="AF10" s="23"/>
       <c r="AG10" s="23"/>
       <c r="AH10" s="24"/>
-    </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="26"/>
+      <c r="AK10" s="26"/>
+      <c r="AL10" s="26"/>
+      <c r="AM10" s="26"/>
+      <c r="AN10" s="26"/>
+      <c r="AO10" s="26"/>
+      <c r="AP10" s="26"/>
+      <c r="AQ10" s="26"/>
+      <c r="AR10" s="26"/>
+      <c r="AS10" s="26"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A11" s="26"/>
       <c r="B11" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="9">
         <v>15</v>
       </c>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="L11" s="14"/>
+      <c r="T11" s="56"/>
       <c r="AH11" s="14"/>
-    </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI11" s="26"/>
+      <c r="AJ11" s="26"/>
+      <c r="AK11" s="26"/>
+      <c r="AL11" s="26"/>
+      <c r="AM11" s="26"/>
+      <c r="AN11" s="26"/>
+      <c r="AO11" s="26"/>
+      <c r="AP11" s="26"/>
+      <c r="AQ11" s="26"/>
+      <c r="AR11" s="26"/>
+      <c r="AS11" s="26"/>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A12" s="26"/>
       <c r="B12" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="9">
         <v>20</v>
       </c>
-      <c r="J12" s="47"/>
-      <c r="K12" s="52"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="14"/>
+      <c r="T12" s="56"/>
       <c r="AH12" s="14"/>
-    </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="26"/>
+      <c r="AL12" s="26"/>
+      <c r="AM12" s="26"/>
+      <c r="AN12" s="26"/>
+      <c r="AO12" s="26"/>
+      <c r="AP12" s="26"/>
+      <c r="AQ12" s="26"/>
+      <c r="AR12" s="26"/>
+      <c r="AS12" s="26"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
       <c r="B13" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="8">
         <v>30</v>
       </c>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="52"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
       <c r="K13" s="52"/>
       <c r="L13" s="14"/>
+      <c r="T13" s="56"/>
       <c r="AH13" s="14"/>
-    </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="26"/>
+      <c r="AL13" s="26"/>
+      <c r="AM13" s="26"/>
+      <c r="AN13" s="26"/>
+      <c r="AO13" s="26"/>
+      <c r="AP13" s="26"/>
+      <c r="AQ13" s="26"/>
+      <c r="AR13" s="26"/>
+      <c r="AS13" s="26"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A14" s="26"/>
       <c r="B14" s="12" t="s">
         <v>33</v>
       </c>
@@ -2469,10 +2783,23 @@
         <v>10</v>
       </c>
       <c r="L14" s="53"/>
-      <c r="M14" s="13"/>
+      <c r="M14" s="52"/>
+      <c r="T14" s="56"/>
       <c r="AH14" s="14"/>
-    </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="26"/>
+      <c r="AK14" s="26"/>
+      <c r="AL14" s="26"/>
+      <c r="AM14" s="26"/>
+      <c r="AN14" s="26"/>
+      <c r="AO14" s="26"/>
+      <c r="AP14" s="26"/>
+      <c r="AQ14" s="26"/>
+      <c r="AR14" s="26"/>
+      <c r="AS14" s="26"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A15" s="26"/>
       <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
@@ -2484,23 +2811,52 @@
       </c>
       <c r="L15" s="14"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="13"/>
+      <c r="O15" s="37"/>
+      <c r="T15" s="56"/>
       <c r="AH15" s="14"/>
-    </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI15" s="26"/>
+      <c r="AJ15" s="26"/>
+      <c r="AK15" s="26"/>
+      <c r="AL15" s="26"/>
+      <c r="AM15" s="26"/>
+      <c r="AN15" s="26"/>
+      <c r="AO15" s="26"/>
+      <c r="AP15" s="26"/>
+      <c r="AQ15" s="26"/>
+      <c r="AR15" s="26"/>
+      <c r="AS15" s="26"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
       <c r="B16" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="C16" s="9">
+        <v>10</v>
+      </c>
       <c r="D16" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L16" s="14"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="63"/>
+      <c r="T16" s="56"/>
       <c r="AH16" s="14"/>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI16" s="26"/>
+      <c r="AJ16" s="26"/>
+      <c r="AK16" s="26"/>
+      <c r="AL16" s="26"/>
+      <c r="AM16" s="26"/>
+      <c r="AN16" s="26"/>
+      <c r="AO16" s="26"/>
+      <c r="AP16" s="26"/>
+      <c r="AQ16" s="26"/>
+      <c r="AR16" s="26"/>
+      <c r="AS16" s="26"/>
+    </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
       <c r="B17" s="12" t="s">
         <v>31</v>
       </c>
@@ -2511,24 +2867,36 @@
         <v>25</v>
       </c>
       <c r="L17" s="14"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="64"/>
       <c r="AH17" s="14"/>
-    </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI17" s="26"/>
+      <c r="AJ17" s="26"/>
+      <c r="AK17" s="26"/>
+      <c r="AL17" s="26"/>
+      <c r="AM17" s="26"/>
+      <c r="AN17" s="26"/>
+      <c r="AO17" s="26"/>
+      <c r="AP17" s="26"/>
+      <c r="AQ17" s="26"/>
+      <c r="AR17" s="26"/>
+      <c r="AS17" s="26"/>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A18" s="26"/>
       <c r="B18" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="21">
         <f>SUM(C11:C17)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D18" s="22">
         <f>SUM(D11:D17)</f>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -2545,7 +2913,7 @@
       <c r="Q18" s="23"/>
       <c r="R18" s="23"/>
       <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
+      <c r="T18" s="57"/>
       <c r="U18" s="21"/>
       <c r="V18" s="23"/>
       <c r="W18" s="23"/>
@@ -2560,8 +2928,20 @@
       <c r="AF18" s="23"/>
       <c r="AG18" s="23"/>
       <c r="AH18" s="24"/>
-    </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI18" s="26"/>
+      <c r="AJ18" s="26"/>
+      <c r="AK18" s="26"/>
+      <c r="AL18" s="26"/>
+      <c r="AM18" s="26"/>
+      <c r="AN18" s="26"/>
+      <c r="AO18" s="26"/>
+      <c r="AP18" s="26"/>
+      <c r="AQ18" s="26"/>
+      <c r="AR18" s="26"/>
+      <c r="AS18" s="26"/>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
       <c r="B19" s="12" t="s">
         <v>34</v>
       </c>
@@ -2572,10 +2952,23 @@
         <v>10</v>
       </c>
       <c r="L19" s="14"/>
+      <c r="T19" s="56"/>
       <c r="V19" s="13"/>
       <c r="AH19" s="14"/>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI19" s="26"/>
+      <c r="AJ19" s="26"/>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="26"/>
+      <c r="AM19" s="26"/>
+      <c r="AN19" s="26"/>
+      <c r="AO19" s="26"/>
+      <c r="AP19" s="26"/>
+      <c r="AQ19" s="26"/>
+      <c r="AR19" s="26"/>
+      <c r="AS19" s="26"/>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A20" s="26"/>
       <c r="B20" s="12" t="s">
         <v>36</v>
       </c>
@@ -2586,10 +2979,23 @@
         <v>10</v>
       </c>
       <c r="L20" s="14"/>
+      <c r="T20" s="56"/>
       <c r="W20" s="13"/>
       <c r="AH20" s="14"/>
-    </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI20" s="26"/>
+      <c r="AJ20" s="26"/>
+      <c r="AK20" s="26"/>
+      <c r="AL20" s="26"/>
+      <c r="AM20" s="26"/>
+      <c r="AN20" s="26"/>
+      <c r="AO20" s="26"/>
+      <c r="AP20" s="26"/>
+      <c r="AQ20" s="26"/>
+      <c r="AR20" s="26"/>
+      <c r="AS20" s="26"/>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A21" s="26"/>
       <c r="B21" s="12" t="s">
         <v>37</v>
       </c>
@@ -2600,10 +3006,23 @@
         <v>8</v>
       </c>
       <c r="L21" s="14"/>
+      <c r="T21" s="56"/>
       <c r="X21" s="13"/>
       <c r="AH21" s="14"/>
-    </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI21" s="26"/>
+      <c r="AJ21" s="26"/>
+      <c r="AK21" s="26"/>
+      <c r="AL21" s="26"/>
+      <c r="AM21" s="26"/>
+      <c r="AN21" s="26"/>
+      <c r="AO21" s="26"/>
+      <c r="AP21" s="26"/>
+      <c r="AQ21" s="26"/>
+      <c r="AR21" s="26"/>
+      <c r="AS21" s="26"/>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
       <c r="B22" s="12" t="s">
         <v>35</v>
       </c>
@@ -2614,10 +3033,23 @@
         <v>5</v>
       </c>
       <c r="L22" s="14"/>
+      <c r="T22" s="56"/>
       <c r="Y22" s="13"/>
       <c r="AH22" s="14"/>
-    </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI22" s="26"/>
+      <c r="AJ22" s="26"/>
+      <c r="AK22" s="26"/>
+      <c r="AL22" s="26"/>
+      <c r="AM22" s="26"/>
+      <c r="AN22" s="26"/>
+      <c r="AO22" s="26"/>
+      <c r="AP22" s="26"/>
+      <c r="AQ22" s="26"/>
+      <c r="AR22" s="26"/>
+      <c r="AS22" s="26"/>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
       <c r="B23" s="20" t="s">
         <v>23</v>
       </c>
@@ -2644,7 +3076,7 @@
       <c r="Q23" s="23"/>
       <c r="R23" s="23"/>
       <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
+      <c r="T23" s="57"/>
       <c r="U23" s="23"/>
       <c r="V23" s="23"/>
       <c r="W23" s="23"/>
@@ -2659,8 +3091,20 @@
       <c r="AF23" s="23"/>
       <c r="AG23" s="23"/>
       <c r="AH23" s="24"/>
-    </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI23" s="26"/>
+      <c r="AJ23" s="26"/>
+      <c r="AK23" s="26"/>
+      <c r="AL23" s="26"/>
+      <c r="AM23" s="26"/>
+      <c r="AN23" s="26"/>
+      <c r="AO23" s="26"/>
+      <c r="AP23" s="26"/>
+      <c r="AQ23" s="26"/>
+      <c r="AR23" s="26"/>
+      <c r="AS23" s="26"/>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
       <c r="B24" s="12" t="s">
         <v>22</v>
       </c>
@@ -2671,13 +3115,26 @@
         <v>30</v>
       </c>
       <c r="L24" s="14"/>
-      <c r="AA24" s="13"/>
+      <c r="T24" s="56"/>
+      <c r="AA24" s="37"/>
       <c r="AB24" s="13"/>
       <c r="AC24" s="13"/>
       <c r="AD24" s="13"/>
       <c r="AH24" s="14"/>
-    </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI24" s="26"/>
+      <c r="AJ24" s="26"/>
+      <c r="AK24" s="26"/>
+      <c r="AL24" s="26"/>
+      <c r="AM24" s="26"/>
+      <c r="AN24" s="26"/>
+      <c r="AO24" s="26"/>
+      <c r="AP24" s="26"/>
+      <c r="AQ24" s="26"/>
+      <c r="AR24" s="26"/>
+      <c r="AS24" s="26"/>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
       <c r="B25" s="12" t="s">
         <v>28</v>
       </c>
@@ -2688,10 +3145,23 @@
         <v>5</v>
       </c>
       <c r="L25" s="14"/>
+      <c r="T25" s="56"/>
       <c r="AE25" s="13"/>
       <c r="AH25" s="14"/>
-    </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI25" s="26"/>
+      <c r="AJ25" s="26"/>
+      <c r="AK25" s="26"/>
+      <c r="AL25" s="26"/>
+      <c r="AM25" s="26"/>
+      <c r="AN25" s="26"/>
+      <c r="AO25" s="26"/>
+      <c r="AP25" s="26"/>
+      <c r="AQ25" s="26"/>
+      <c r="AR25" s="26"/>
+      <c r="AS25" s="26"/>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
       <c r="B26" s="20" t="s">
         <v>21</v>
       </c>
@@ -2718,7 +3188,7 @@
       <c r="Q26" s="23"/>
       <c r="R26" s="23"/>
       <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
+      <c r="T26" s="57"/>
       <c r="U26" s="23"/>
       <c r="V26" s="23"/>
       <c r="W26" s="23"/>
@@ -2733,18 +3203,30 @@
       <c r="AF26" s="21"/>
       <c r="AG26" s="21"/>
       <c r="AH26" s="25"/>
-    </row>
-    <row r="27" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AI26" s="26"/>
+      <c r="AJ26" s="26"/>
+      <c r="AK26" s="26"/>
+      <c r="AL26" s="26"/>
+      <c r="AM26" s="26"/>
+      <c r="AN26" s="26"/>
+      <c r="AO26" s="26"/>
+      <c r="AP26" s="26"/>
+      <c r="AQ26" s="26"/>
+      <c r="AR26" s="26"/>
+      <c r="AS26" s="26"/>
+    </row>
+    <row r="27" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="26"/>
       <c r="B27" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="16">
         <f>C7+C10+C18+C26+C23</f>
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D27" s="17">
         <f>D7+D10+D18+D26+D23</f>
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
@@ -2761,7 +3243,7 @@
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
       <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
+      <c r="T27" s="58"/>
       <c r="U27" s="18"/>
       <c r="V27" s="18"/>
       <c r="W27" s="18"/>
@@ -2776,859 +3258,1945 @@
       <c r="AF27" s="18"/>
       <c r="AG27" s="18"/>
       <c r="AH27" s="19"/>
-    </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="D28" s="9"/>
-      <c r="K28" t="s">
+      <c r="AI27" s="26"/>
+      <c r="AJ27" s="26"/>
+      <c r="AK27" s="26"/>
+      <c r="AL27" s="26"/>
+      <c r="AM27" s="26"/>
+      <c r="AN27" s="26"/>
+      <c r="AO27" s="26"/>
+      <c r="AP27" s="26"/>
+      <c r="AQ27" s="26"/>
+      <c r="AR27" s="26"/>
+      <c r="AS27" s="26"/>
+    </row>
+    <row r="28" spans="1:45" ht="16.149999999999999" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="AH28"/>
-    </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="D29" s="9"/>
-      <c r="AH29"/>
-    </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="D30" s="9"/>
-      <c r="AH30"/>
-    </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="D31" s="9"/>
-      <c r="AH31"/>
-    </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="D32" s="9"/>
-      <c r="AH32"/>
-    </row>
-    <row r="33" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-    </row>
-    <row r="34" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-    </row>
-    <row r="39" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-    </row>
-    <row r="40" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-    </row>
-    <row r="41" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="42" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-    </row>
-    <row r="44" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-    </row>
-    <row r="45" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-    </row>
-    <row r="46" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-    </row>
-    <row r="47" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-    </row>
-    <row r="49" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="26"/>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="26"/>
+      <c r="AE28" s="26"/>
+      <c r="AF28" s="26"/>
+      <c r="AG28" s="26"/>
+      <c r="AH28" s="26"/>
+      <c r="AI28" s="26"/>
+      <c r="AJ28" s="26"/>
+      <c r="AK28" s="26"/>
+      <c r="AL28" s="26"/>
+      <c r="AM28" s="26"/>
+      <c r="AN28" s="26"/>
+      <c r="AO28" s="26"/>
+      <c r="AP28" s="26"/>
+      <c r="AQ28" s="26"/>
+      <c r="AR28" s="26"/>
+      <c r="AS28" s="26"/>
+    </row>
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="26"/>
+      <c r="AC29" s="26"/>
+      <c r="AD29" s="26"/>
+      <c r="AE29" s="26"/>
+      <c r="AF29" s="26"/>
+      <c r="AG29" s="26"/>
+      <c r="AH29" s="26"/>
+      <c r="AI29" s="26"/>
+      <c r="AJ29" s="26"/>
+      <c r="AK29" s="26"/>
+      <c r="AL29" s="26"/>
+      <c r="AM29" s="26"/>
+      <c r="AN29" s="26"/>
+      <c r="AO29" s="26"/>
+      <c r="AP29" s="26"/>
+      <c r="AQ29" s="26"/>
+      <c r="AR29" s="26"/>
+      <c r="AS29" s="26"/>
+    </row>
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="26"/>
+      <c r="AD30" s="26"/>
+      <c r="AE30" s="26"/>
+      <c r="AF30" s="26"/>
+      <c r="AG30" s="26"/>
+      <c r="AH30" s="26"/>
+      <c r="AI30" s="26"/>
+      <c r="AJ30" s="26"/>
+      <c r="AK30" s="26"/>
+      <c r="AL30" s="26"/>
+      <c r="AM30" s="26"/>
+      <c r="AN30" s="26"/>
+      <c r="AO30" s="26"/>
+      <c r="AP30" s="26"/>
+      <c r="AQ30" s="26"/>
+      <c r="AR30" s="26"/>
+      <c r="AS30" s="26"/>
+    </row>
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+      <c r="Y31" s="26"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="26"/>
+      <c r="AB31" s="26"/>
+      <c r="AC31" s="26"/>
+      <c r="AD31" s="26"/>
+      <c r="AE31" s="26"/>
+      <c r="AF31" s="26"/>
+      <c r="AG31" s="26"/>
+      <c r="AH31" s="26"/>
+      <c r="AI31" s="26"/>
+      <c r="AJ31" s="26"/>
+      <c r="AK31" s="26"/>
+      <c r="AL31" s="26"/>
+      <c r="AM31" s="26"/>
+      <c r="AN31" s="26"/>
+      <c r="AO31" s="26"/>
+      <c r="AP31" s="26"/>
+      <c r="AQ31" s="26"/>
+      <c r="AR31" s="26"/>
+      <c r="AS31" s="26"/>
+    </row>
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="26"/>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="26"/>
+      <c r="AF32" s="26"/>
+      <c r="AG32" s="26"/>
+      <c r="AH32" s="26"/>
+      <c r="AI32" s="26"/>
+      <c r="AJ32" s="26"/>
+      <c r="AK32" s="26"/>
+      <c r="AL32" s="26"/>
+      <c r="AM32" s="26"/>
+      <c r="AN32" s="26"/>
+      <c r="AO32" s="26"/>
+      <c r="AP32" s="26"/>
+      <c r="AQ32" s="26"/>
+      <c r="AR32" s="26"/>
+      <c r="AS32" s="26"/>
+    </row>
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="26"/>
+      <c r="AC33" s="26"/>
+      <c r="AD33" s="26"/>
+      <c r="AE33" s="26"/>
+      <c r="AF33" s="26"/>
+      <c r="AG33" s="26"/>
+      <c r="AH33" s="26"/>
+      <c r="AI33" s="26"/>
+      <c r="AJ33" s="26"/>
+      <c r="AK33" s="26"/>
+      <c r="AL33" s="26"/>
+      <c r="AM33" s="26"/>
+      <c r="AN33" s="26"/>
+      <c r="AO33" s="26"/>
+      <c r="AP33" s="26"/>
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="26"/>
+    </row>
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+      <c r="Y34" s="26"/>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="26"/>
+      <c r="AC34" s="26"/>
+      <c r="AD34" s="26"/>
+      <c r="AE34" s="26"/>
+      <c r="AF34" s="26"/>
+      <c r="AG34" s="26"/>
+      <c r="AH34" s="26"/>
+      <c r="AI34" s="26"/>
+      <c r="AJ34" s="26"/>
+      <c r="AK34" s="26"/>
+      <c r="AL34" s="26"/>
+      <c r="AM34" s="26"/>
+      <c r="AN34" s="26"/>
+      <c r="AO34" s="26"/>
+      <c r="AP34" s="26"/>
+      <c r="AQ34" s="26"/>
+      <c r="AR34" s="26"/>
+      <c r="AS34" s="26"/>
+    </row>
+    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="26"/>
+      <c r="Y35" s="26"/>
+      <c r="Z35" s="26"/>
+      <c r="AA35" s="26"/>
+      <c r="AB35" s="26"/>
+      <c r="AC35" s="26"/>
+      <c r="AD35" s="26"/>
+      <c r="AE35" s="26"/>
+      <c r="AF35" s="26"/>
+      <c r="AG35" s="26"/>
+      <c r="AH35" s="26"/>
+      <c r="AI35" s="26"/>
+      <c r="AJ35" s="26"/>
+      <c r="AK35" s="26"/>
+      <c r="AL35" s="26"/>
+      <c r="AM35" s="26"/>
+      <c r="AN35" s="26"/>
+      <c r="AO35" s="26"/>
+      <c r="AP35" s="26"/>
+      <c r="AQ35" s="26"/>
+      <c r="AR35" s="26"/>
+      <c r="AS35" s="26"/>
+    </row>
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="26"/>
+      <c r="Y36" s="26"/>
+      <c r="Z36" s="26"/>
+      <c r="AA36" s="26"/>
+      <c r="AB36" s="26"/>
+      <c r="AC36" s="26"/>
+      <c r="AD36" s="26"/>
+      <c r="AE36" s="26"/>
+      <c r="AF36" s="26"/>
+      <c r="AG36" s="26"/>
+      <c r="AH36" s="26"/>
+      <c r="AI36" s="26"/>
+      <c r="AJ36" s="26"/>
+      <c r="AK36" s="26"/>
+      <c r="AL36" s="26"/>
+      <c r="AM36" s="26"/>
+      <c r="AN36" s="26"/>
+      <c r="AO36" s="26"/>
+      <c r="AP36" s="26"/>
+      <c r="AQ36" s="26"/>
+      <c r="AR36" s="26"/>
+      <c r="AS36" s="26"/>
+    </row>
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
+      <c r="Y37" s="26"/>
+      <c r="Z37" s="26"/>
+      <c r="AA37" s="26"/>
+      <c r="AB37" s="26"/>
+      <c r="AC37" s="26"/>
+      <c r="AD37" s="26"/>
+      <c r="AE37" s="26"/>
+      <c r="AF37" s="26"/>
+      <c r="AG37" s="26"/>
+      <c r="AH37" s="26"/>
+      <c r="AI37" s="26"/>
+      <c r="AJ37" s="26"/>
+      <c r="AK37" s="26"/>
+      <c r="AL37" s="26"/>
+      <c r="AM37" s="26"/>
+      <c r="AN37" s="26"/>
+      <c r="AO37" s="26"/>
+      <c r="AP37" s="26"/>
+      <c r="AQ37" s="26"/>
+      <c r="AR37" s="26"/>
+      <c r="AS37" s="26"/>
+    </row>
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
+      <c r="Y38" s="26"/>
+      <c r="Z38" s="26"/>
+      <c r="AA38" s="26"/>
+      <c r="AB38" s="26"/>
+      <c r="AC38" s="26"/>
+      <c r="AD38" s="26"/>
+      <c r="AE38" s="26"/>
+      <c r="AF38" s="26"/>
+      <c r="AG38" s="26"/>
+      <c r="AH38" s="26"/>
+      <c r="AI38" s="26"/>
+      <c r="AJ38" s="26"/>
+      <c r="AK38" s="26"/>
+      <c r="AL38" s="26"/>
+      <c r="AM38" s="26"/>
+      <c r="AN38" s="26"/>
+      <c r="AO38" s="26"/>
+      <c r="AP38" s="26"/>
+      <c r="AQ38" s="26"/>
+      <c r="AR38" s="26"/>
+      <c r="AS38" s="26"/>
+    </row>
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="26"/>
+      <c r="AB39" s="26"/>
+      <c r="AC39" s="26"/>
+      <c r="AD39" s="26"/>
+      <c r="AE39" s="26"/>
+      <c r="AF39" s="26"/>
+      <c r="AG39" s="26"/>
+      <c r="AH39" s="26"/>
+      <c r="AI39" s="26"/>
+      <c r="AJ39" s="26"/>
+      <c r="AK39" s="26"/>
+      <c r="AL39" s="26"/>
+      <c r="AM39" s="26"/>
+      <c r="AN39" s="26"/>
+      <c r="AO39" s="26"/>
+      <c r="AP39" s="26"/>
+      <c r="AQ39" s="26"/>
+      <c r="AR39" s="26"/>
+      <c r="AS39" s="26"/>
+    </row>
+    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+      <c r="AB40" s="26"/>
+      <c r="AC40" s="26"/>
+      <c r="AD40" s="26"/>
+      <c r="AE40" s="26"/>
+      <c r="AF40" s="26"/>
+      <c r="AG40" s="26"/>
+      <c r="AH40" s="26"/>
+      <c r="AI40" s="26"/>
+      <c r="AJ40" s="26"/>
+      <c r="AK40" s="26"/>
+      <c r="AL40" s="26"/>
+      <c r="AM40" s="26"/>
+      <c r="AN40" s="26"/>
+      <c r="AO40" s="26"/>
+      <c r="AP40" s="26"/>
+      <c r="AQ40" s="26"/>
+      <c r="AR40" s="26"/>
+      <c r="AS40" s="26"/>
+    </row>
+    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="26"/>
+      <c r="AC41" s="26"/>
+      <c r="AD41" s="26"/>
+      <c r="AE41" s="26"/>
+      <c r="AF41" s="26"/>
+      <c r="AG41" s="26"/>
+      <c r="AH41" s="26"/>
+      <c r="AI41" s="26"/>
+      <c r="AJ41" s="26"/>
+      <c r="AK41" s="26"/>
+      <c r="AL41" s="26"/>
+      <c r="AM41" s="26"/>
+      <c r="AN41" s="26"/>
+      <c r="AO41" s="26"/>
+      <c r="AP41" s="26"/>
+      <c r="AQ41" s="26"/>
+      <c r="AR41" s="26"/>
+      <c r="AS41" s="26"/>
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="26"/>
+      <c r="T42" s="26"/>
+      <c r="U42" s="26"/>
+      <c r="V42" s="26"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="26"/>
+      <c r="Z42" s="26"/>
+      <c r="AA42" s="26"/>
+      <c r="AB42" s="26"/>
+      <c r="AC42" s="26"/>
+      <c r="AD42" s="26"/>
+      <c r="AE42" s="26"/>
+      <c r="AF42" s="26"/>
+      <c r="AG42" s="26"/>
+      <c r="AH42" s="26"/>
+      <c r="AI42" s="26"/>
+      <c r="AJ42" s="26"/>
+      <c r="AK42" s="26"/>
+      <c r="AL42" s="26"/>
+      <c r="AM42" s="26"/>
+      <c r="AN42" s="26"/>
+      <c r="AO42" s="26"/>
+      <c r="AP42" s="26"/>
+      <c r="AQ42" s="26"/>
+      <c r="AR42" s="26"/>
+      <c r="AS42" s="26"/>
+    </row>
+    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="26"/>
+      <c r="T43" s="26"/>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+      <c r="Y43" s="26"/>
+      <c r="Z43" s="26"/>
+      <c r="AA43" s="26"/>
+      <c r="AB43" s="26"/>
+      <c r="AC43" s="26"/>
+      <c r="AD43" s="26"/>
+      <c r="AE43" s="26"/>
+      <c r="AF43" s="26"/>
+      <c r="AG43" s="26"/>
+      <c r="AH43" s="26"/>
+      <c r="AI43" s="26"/>
+      <c r="AJ43" s="26"/>
+      <c r="AK43" s="26"/>
+      <c r="AL43" s="26"/>
+      <c r="AM43" s="26"/>
+      <c r="AN43" s="26"/>
+      <c r="AO43" s="26"/>
+      <c r="AP43" s="26"/>
+      <c r="AQ43" s="26"/>
+      <c r="AR43" s="26"/>
+      <c r="AS43" s="26"/>
+    </row>
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="26"/>
+      <c r="T44" s="26"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26"/>
+      <c r="Y44" s="26"/>
+      <c r="Z44" s="26"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="26"/>
+      <c r="AC44" s="26"/>
+      <c r="AD44" s="26"/>
+      <c r="AE44" s="26"/>
+      <c r="AF44" s="26"/>
+      <c r="AG44" s="26"/>
+      <c r="AH44" s="26"/>
+      <c r="AI44" s="26"/>
+      <c r="AJ44" s="26"/>
+      <c r="AK44" s="26"/>
+      <c r="AL44" s="26"/>
+      <c r="AM44" s="26"/>
+      <c r="AN44" s="26"/>
+      <c r="AO44" s="26"/>
+      <c r="AP44" s="26"/>
+      <c r="AQ44" s="26"/>
+      <c r="AR44" s="26"/>
+      <c r="AS44" s="26"/>
+    </row>
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="26"/>
+      <c r="T45" s="26"/>
+      <c r="U45" s="26"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
+      <c r="Y45" s="26"/>
+      <c r="Z45" s="26"/>
+      <c r="AA45" s="26"/>
+      <c r="AB45" s="26"/>
+      <c r="AC45" s="26"/>
+      <c r="AD45" s="26"/>
+      <c r="AE45" s="26"/>
+      <c r="AF45" s="26"/>
+      <c r="AG45" s="26"/>
+      <c r="AH45" s="26"/>
+      <c r="AI45" s="26"/>
+      <c r="AJ45" s="26"/>
+      <c r="AK45" s="26"/>
+      <c r="AL45" s="26"/>
+      <c r="AM45" s="26"/>
+      <c r="AN45" s="26"/>
+      <c r="AO45" s="26"/>
+      <c r="AP45" s="26"/>
+      <c r="AQ45" s="26"/>
+      <c r="AR45" s="26"/>
+      <c r="AS45" s="26"/>
+    </row>
+    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
+      <c r="P46" s="26"/>
+      <c r="Q46" s="26"/>
+      <c r="R46" s="26"/>
+      <c r="S46" s="26"/>
+      <c r="T46" s="26"/>
+      <c r="U46" s="26"/>
+      <c r="V46" s="26"/>
+      <c r="W46" s="26"/>
+      <c r="X46" s="26"/>
+      <c r="Y46" s="26"/>
+      <c r="Z46" s="26"/>
+      <c r="AA46" s="26"/>
+      <c r="AB46" s="26"/>
+      <c r="AC46" s="26"/>
+      <c r="AD46" s="26"/>
+      <c r="AE46" s="26"/>
+      <c r="AF46" s="26"/>
+      <c r="AG46" s="26"/>
+      <c r="AH46" s="26"/>
+      <c r="AI46" s="26"/>
+      <c r="AJ46" s="26"/>
+      <c r="AK46" s="26"/>
+      <c r="AL46" s="26"/>
+      <c r="AM46" s="26"/>
+      <c r="AN46" s="26"/>
+      <c r="AO46" s="26"/>
+      <c r="AP46" s="26"/>
+      <c r="AQ46" s="26"/>
+      <c r="AR46" s="26"/>
+      <c r="AS46" s="26"/>
+    </row>
+    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="26"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="26"/>
+      <c r="T47" s="26"/>
+      <c r="U47" s="26"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="26"/>
+      <c r="X47" s="26"/>
+      <c r="Y47" s="26"/>
+      <c r="Z47" s="26"/>
+      <c r="AA47" s="26"/>
+      <c r="AB47" s="26"/>
+      <c r="AC47" s="26"/>
+      <c r="AD47" s="26"/>
+      <c r="AE47" s="26"/>
+      <c r="AF47" s="26"/>
+      <c r="AG47" s="26"/>
+      <c r="AH47" s="26"/>
+      <c r="AI47" s="26"/>
+      <c r="AJ47" s="26"/>
+      <c r="AK47" s="26"/>
+      <c r="AL47" s="26"/>
+      <c r="AM47" s="26"/>
+      <c r="AN47" s="26"/>
+      <c r="AO47" s="26"/>
+      <c r="AP47" s="26"/>
+      <c r="AQ47" s="26"/>
+      <c r="AR47" s="26"/>
+      <c r="AS47" s="26"/>
+    </row>
+    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="26"/>
+      <c r="R48" s="26"/>
+      <c r="S48" s="26"/>
+      <c r="T48" s="26"/>
+      <c r="U48" s="26"/>
+      <c r="V48" s="26"/>
+      <c r="W48" s="26"/>
+      <c r="X48" s="26"/>
+      <c r="Y48" s="26"/>
+      <c r="Z48" s="26"/>
+      <c r="AA48" s="26"/>
+      <c r="AB48" s="26"/>
+      <c r="AC48" s="26"/>
+      <c r="AD48" s="26"/>
+      <c r="AE48" s="26"/>
+      <c r="AF48" s="26"/>
+      <c r="AG48" s="26"/>
+      <c r="AH48" s="26"/>
+      <c r="AI48" s="26"/>
+      <c r="AJ48" s="26"/>
+      <c r="AK48" s="26"/>
+      <c r="AL48" s="26"/>
+    </row>
+    <row r="49" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="26"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
     </row>
-    <row r="50" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="26"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
     </row>
-    <row r="51" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="26"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
     </row>
-    <row r="52" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="26"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
     </row>
-    <row r="53" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="26"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
     </row>
-    <row r="54" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="26"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
     </row>
-    <row r="55" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="26"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
     </row>
-    <row r="56" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="26"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
     </row>
-    <row r="57" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="26"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
     </row>
-    <row r="58" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="26"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
     </row>
-    <row r="59" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="26"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
     </row>
-    <row r="60" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="26"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
     </row>
-    <row r="61" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="26"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="26"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="26"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
     </row>
-    <row r="64" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="26"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
     </row>
-    <row r="65" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="26"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
     </row>
-    <row r="66" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="26"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
     </row>
-    <row r="67" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="26"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
     </row>
-    <row r="68" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="26"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
     </row>
-    <row r="69" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="26"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
     </row>
-    <row r="70" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="26"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
     </row>
-    <row r="71" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="26"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
     </row>
-    <row r="72" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="26"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
     </row>
-    <row r="73" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="26"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
     </row>
-    <row r="74" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="26"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
     </row>
-    <row r="75" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="26"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
     </row>
-    <row r="76" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="26"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
     </row>
-    <row r="77" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="26"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
     </row>
-    <row r="78" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="26"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
     </row>
-    <row r="79" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="26"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
     </row>
-    <row r="80" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="26"/>
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
     </row>
-    <row r="81" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="26"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
     </row>
-    <row r="82" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="26"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
     </row>
-    <row r="83" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="26"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
     </row>
-    <row r="84" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="26"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
     </row>
-    <row r="85" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="26"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
     </row>
-    <row r="86" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="26"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
     </row>
-    <row r="87" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="26"/>
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
     </row>
-    <row r="88" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="26"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
     </row>
-    <row r="89" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="26"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
     </row>
-    <row r="90" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="26"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
     </row>
-    <row r="91" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="26"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
     </row>
-    <row r="92" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="26"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
     </row>
-    <row r="93" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="26"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
     </row>
-    <row r="94" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="26"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
     </row>
-    <row r="95" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="26"/>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
     </row>
-    <row r="96" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="26"/>
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
     </row>
-    <row r="97" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="26"/>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
     </row>
-    <row r="98" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="26"/>
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
     </row>
-    <row r="99" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="26"/>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
     </row>
-    <row r="100" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="26"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
     </row>
-    <row r="101" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="26"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
     </row>
-    <row r="102" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="26"/>
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
     </row>
-    <row r="103" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="26"/>
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
     </row>
-    <row r="104" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="26"/>
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
     </row>
-    <row r="105" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="26"/>
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
     </row>
-    <row r="106" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="26"/>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
     </row>
-    <row r="107" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="26"/>
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
     </row>
-    <row r="108" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="26"/>
       <c r="C108" s="9"/>
       <c r="D108" s="9"/>
     </row>
-    <row r="109" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="26"/>
       <c r="C109" s="9"/>
       <c r="D109" s="9"/>
     </row>
-    <row r="110" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="26"/>
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
     </row>
-    <row r="111" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="26"/>
       <c r="C111" s="9"/>
       <c r="D111" s="9"/>
     </row>
-    <row r="112" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="26"/>
       <c r="C112" s="9"/>
       <c r="D112" s="9"/>
     </row>
-    <row r="113" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="26"/>
       <c r="C113" s="9"/>
       <c r="D113" s="9"/>
     </row>
-    <row r="114" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="26"/>
       <c r="C114" s="9"/>
       <c r="D114" s="9"/>
     </row>
-    <row r="115" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="26"/>
       <c r="C115" s="9"/>
       <c r="D115" s="9"/>
     </row>
-    <row r="116" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="26"/>
       <c r="C116" s="9"/>
       <c r="D116" s="9"/>
     </row>
-    <row r="117" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="26"/>
       <c r="C117" s="9"/>
       <c r="D117" s="9"/>
     </row>
-    <row r="118" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="26"/>
       <c r="C118" s="9"/>
       <c r="D118" s="9"/>
     </row>
-    <row r="119" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="26"/>
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
     </row>
-    <row r="120" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="26"/>
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
     </row>
-    <row r="121" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="26"/>
       <c r="C121" s="9"/>
       <c r="D121" s="9"/>
     </row>
-    <row r="122" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="26"/>
       <c r="C122" s="9"/>
       <c r="D122" s="9"/>
     </row>
-    <row r="123" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="26"/>
       <c r="C123" s="9"/>
       <c r="D123" s="9"/>
     </row>
-    <row r="124" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="26"/>
       <c r="C124" s="9"/>
       <c r="D124" s="9"/>
     </row>
-    <row r="125" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="26"/>
       <c r="C125" s="9"/>
       <c r="D125" s="9"/>
     </row>
-    <row r="126" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="26"/>
       <c r="C126" s="9"/>
       <c r="D126" s="9"/>
     </row>
-    <row r="127" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="26"/>
       <c r="C127" s="9"/>
       <c r="D127" s="9"/>
     </row>
-    <row r="128" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="26"/>
       <c r="C128" s="9"/>
       <c r="D128" s="9"/>
     </row>
-    <row r="129" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="26"/>
       <c r="C129" s="9"/>
       <c r="D129" s="9"/>
     </row>
-    <row r="130" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="26"/>
       <c r="C130" s="9"/>
       <c r="D130" s="9"/>
     </row>
-    <row r="131" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="26"/>
       <c r="C131" s="9"/>
       <c r="D131" s="9"/>
     </row>
-    <row r="132" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="26"/>
       <c r="C132" s="9"/>
       <c r="D132" s="9"/>
     </row>
-    <row r="133" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="26"/>
       <c r="C133" s="9"/>
       <c r="D133" s="9"/>
     </row>
-    <row r="134" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="26"/>
       <c r="C134" s="9"/>
       <c r="D134" s="9"/>
     </row>
-    <row r="135" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="26"/>
       <c r="C135" s="9"/>
       <c r="D135" s="9"/>
     </row>
-    <row r="136" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="26"/>
       <c r="C136" s="9"/>
       <c r="D136" s="9"/>
     </row>
-    <row r="137" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="26"/>
       <c r="C137" s="9"/>
       <c r="D137" s="9"/>
     </row>
-    <row r="138" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="26"/>
       <c r="C138" s="9"/>
       <c r="D138" s="9"/>
     </row>
-    <row r="139" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="26"/>
       <c r="C139" s="9"/>
       <c r="D139" s="9"/>
     </row>
-    <row r="140" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="26"/>
       <c r="C140" s="9"/>
       <c r="D140" s="9"/>
     </row>
-    <row r="141" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="26"/>
       <c r="C141" s="9"/>
       <c r="D141" s="9"/>
     </row>
-    <row r="142" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="26"/>
       <c r="C142" s="9"/>
       <c r="D142" s="9"/>
     </row>
-    <row r="143" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="26"/>
       <c r="C143" s="9"/>
       <c r="D143" s="9"/>
     </row>
-    <row r="144" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="26"/>
       <c r="C144" s="9"/>
       <c r="D144" s="9"/>
     </row>
-    <row r="145" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="26"/>
       <c r="C145" s="9"/>
       <c r="D145" s="9"/>
     </row>
-    <row r="146" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="26"/>
       <c r="C146" s="9"/>
       <c r="D146" s="9"/>
     </row>
-    <row r="147" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="26"/>
       <c r="C147" s="9"/>
       <c r="D147" s="9"/>
     </row>
-    <row r="148" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="26"/>
       <c r="C148" s="9"/>
       <c r="D148" s="9"/>
     </row>
-    <row r="149" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="26"/>
       <c r="C149" s="9"/>
       <c r="D149" s="9"/>
     </row>
-    <row r="150" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="26"/>
       <c r="C150" s="9"/>
       <c r="D150" s="9"/>
     </row>
-    <row r="151" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="26"/>
       <c r="C151" s="9"/>
       <c r="D151" s="9"/>
     </row>
-    <row r="152" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="26"/>
       <c r="C152" s="9"/>
       <c r="D152" s="9"/>
     </row>
-    <row r="153" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="26"/>
       <c r="C153" s="9"/>
       <c r="D153" s="9"/>
     </row>
-    <row r="154" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="26"/>
       <c r="C154" s="9"/>
       <c r="D154" s="9"/>
     </row>
-    <row r="155" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="26"/>
       <c r="C155" s="9"/>
       <c r="D155" s="9"/>
     </row>
-    <row r="156" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="26"/>
       <c r="C156" s="9"/>
       <c r="D156" s="9"/>
     </row>
-    <row r="157" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="26"/>
       <c r="C157" s="9"/>
       <c r="D157" s="9"/>
     </row>
-    <row r="158" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="26"/>
       <c r="C158" s="9"/>
       <c r="D158" s="9"/>
     </row>
-    <row r="159" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="26"/>
       <c r="C159" s="9"/>
       <c r="D159" s="9"/>
     </row>
-    <row r="160" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="26"/>
       <c r="C160" s="9"/>
       <c r="D160" s="9"/>
     </row>
-    <row r="161" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="26"/>
       <c r="C161" s="9"/>
       <c r="D161" s="9"/>
     </row>
-    <row r="162" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="26"/>
       <c r="C162" s="9"/>
       <c r="D162" s="9"/>
     </row>
-    <row r="163" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="26"/>
       <c r="C163" s="9"/>
       <c r="D163" s="9"/>
     </row>
-    <row r="164" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="26"/>
       <c r="C164" s="9"/>
       <c r="D164" s="9"/>
     </row>
-    <row r="165" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="26"/>
       <c r="C165" s="9"/>
       <c r="D165" s="9"/>
     </row>
-    <row r="166" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="26"/>
       <c r="C166" s="9"/>
       <c r="D166" s="9"/>
     </row>
-    <row r="167" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="26"/>
       <c r="C167" s="9"/>
       <c r="D167" s="9"/>
     </row>
-    <row r="168" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="26"/>
       <c r="C168" s="9"/>
       <c r="D168" s="9"/>
     </row>
-    <row r="169" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="26"/>
       <c r="C169" s="9"/>
       <c r="D169" s="9"/>
     </row>
-    <row r="170" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="26"/>
       <c r="C170" s="9"/>
       <c r="D170" s="9"/>
     </row>
-    <row r="171" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="26"/>
       <c r="C171" s="9"/>
       <c r="D171" s="9"/>
     </row>
-    <row r="172" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="26"/>
       <c r="C172" s="9"/>
       <c r="D172" s="9"/>
     </row>
-    <row r="173" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="26"/>
       <c r="C173" s="9"/>
       <c r="D173" s="9"/>
     </row>
-    <row r="174" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="26"/>
       <c r="C174" s="9"/>
       <c r="D174" s="9"/>
     </row>
-    <row r="175" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="26"/>
       <c r="C175" s="9"/>
       <c r="D175" s="9"/>
     </row>
-    <row r="176" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="26"/>
       <c r="C176" s="9"/>
       <c r="D176" s="9"/>
     </row>
-    <row r="177" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="26"/>
       <c r="C177" s="9"/>
       <c r="D177" s="9"/>
     </row>
-    <row r="178" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="26"/>
       <c r="C178" s="9"/>
       <c r="D178" s="9"/>
     </row>
-    <row r="179" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="26"/>
       <c r="C179" s="9"/>
       <c r="D179" s="9"/>
     </row>
-    <row r="180" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="26"/>
       <c r="C180" s="9"/>
       <c r="D180" s="9"/>
     </row>
-    <row r="181" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="26"/>
       <c r="C181" s="9"/>
       <c r="D181" s="9"/>
     </row>
-    <row r="182" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="26"/>
       <c r="C182" s="9"/>
       <c r="D182" s="9"/>
     </row>
-    <row r="183" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="26"/>
       <c r="C183" s="9"/>
       <c r="D183" s="9"/>
     </row>
-    <row r="184" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="26"/>
       <c r="C184" s="9"/>
       <c r="D184" s="9"/>
     </row>
-    <row r="185" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="26"/>
       <c r="C185" s="9"/>
       <c r="D185" s="9"/>
     </row>
-    <row r="186" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="26"/>
       <c r="C186" s="9"/>
       <c r="D186" s="9"/>
     </row>
-    <row r="187" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="26"/>
       <c r="C187" s="9"/>
       <c r="D187" s="9"/>
     </row>
-    <row r="188" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="26"/>
       <c r="C188" s="9"/>
       <c r="D188" s="9"/>
     </row>
-    <row r="189" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="26"/>
       <c r="C189" s="9"/>
       <c r="D189" s="9"/>
     </row>
-    <row r="190" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="26"/>
       <c r="C190" s="9"/>
       <c r="D190" s="9"/>
     </row>
-    <row r="191" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="26"/>
       <c r="C191" s="9"/>
       <c r="D191" s="9"/>
     </row>
-    <row r="192" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="26"/>
       <c r="C192" s="9"/>
       <c r="D192" s="9"/>
     </row>
-    <row r="193" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="26"/>
       <c r="C193" s="9"/>
       <c r="D193" s="9"/>
     </row>
-    <row r="194" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="26"/>
       <c r="C194" s="9"/>
       <c r="D194" s="9"/>
     </row>
-    <row r="195" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="26"/>
       <c r="C195" s="9"/>
       <c r="D195" s="9"/>
     </row>
-    <row r="196" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="26"/>
       <c r="C196" s="9"/>
       <c r="D196" s="9"/>
     </row>
-    <row r="197" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="26"/>
       <c r="C197" s="9"/>
       <c r="D197" s="9"/>
     </row>
-    <row r="198" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="26"/>
       <c r="C198" s="9"/>
       <c r="D198" s="9"/>
     </row>
-    <row r="199" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="26"/>
       <c r="C199" s="9"/>
       <c r="D199" s="9"/>
     </row>
-    <row r="200" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="26"/>
       <c r="C200" s="9"/>
       <c r="D200" s="9"/>
     </row>
-    <row r="201" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="26"/>
       <c r="C201" s="9"/>
       <c r="D201" s="9"/>
     </row>
-    <row r="202" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="26"/>
       <c r="C202" s="9"/>
       <c r="D202" s="9"/>
     </row>
-    <row r="203" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="26"/>
       <c r="C203" s="9"/>
       <c r="D203" s="9"/>
     </row>
-    <row r="204" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="26"/>
       <c r="C204" s="9"/>
       <c r="D204" s="9"/>
     </row>
-    <row r="205" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="26"/>
       <c r="C205" s="9"/>
       <c r="D205" s="9"/>
     </row>
-    <row r="206" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="26"/>
       <c r="C206" s="9"/>
       <c r="D206" s="9"/>
     </row>
-    <row r="207" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="26"/>
       <c r="C207" s="9"/>
       <c r="D207" s="9"/>
     </row>
-    <row r="208" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="26"/>
       <c r="C208" s="9"/>
       <c r="D208" s="9"/>
     </row>
-    <row r="209" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="26"/>
       <c r="C209" s="9"/>
       <c r="D209" s="9"/>
     </row>
-    <row r="210" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="26"/>
       <c r="C210" s="9"/>
       <c r="D210" s="9"/>
     </row>
-    <row r="211" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="26"/>
       <c r="C211" s="9"/>
       <c r="D211" s="9"/>
     </row>
-    <row r="212" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="26"/>
       <c r="C212" s="9"/>
       <c r="D212" s="9"/>
     </row>
-    <row r="213" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="26"/>
       <c r="C213" s="9"/>
       <c r="D213" s="9"/>
     </row>
-    <row r="214" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="26"/>
       <c r="C214" s="9"/>
       <c r="D214" s="9"/>
     </row>
-    <row r="215" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="26"/>
       <c r="C215" s="9"/>
       <c r="D215" s="9"/>
     </row>
-    <row r="216" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="26"/>
       <c r="C216" s="9"/>
       <c r="D216" s="9"/>
     </row>
-    <row r="217" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="26"/>
       <c r="C217" s="9"/>
       <c r="D217" s="9"/>
     </row>
-    <row r="218" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="26"/>
       <c r="C218" s="9"/>
       <c r="D218" s="9"/>
     </row>
-    <row r="219" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="26"/>
       <c r="C219" s="9"/>
       <c r="D219" s="9"/>
     </row>
-    <row r="220" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="26"/>
       <c r="C220" s="9"/>
       <c r="D220" s="9"/>
     </row>
-    <row r="221" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="26"/>
       <c r="C221" s="9"/>
       <c r="D221" s="9"/>
     </row>
-    <row r="222" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="26"/>
       <c r="C222" s="9"/>
       <c r="D222" s="9"/>
     </row>
-    <row r="223" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="26"/>
       <c r="C223" s="9"/>
       <c r="D223" s="9"/>
     </row>
-    <row r="224" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="26"/>
       <c r="C224" s="9"/>
       <c r="D224" s="9"/>
     </row>
-    <row r="225" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="26"/>
       <c r="C225" s="9"/>
       <c r="D225" s="9"/>
     </row>
-    <row r="226" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="26"/>
       <c r="C226" s="9"/>
       <c r="D226" s="9"/>
     </row>
-    <row r="227" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C227" s="9"/>
       <c r="D227" s="9"/>
     </row>
-    <row r="228" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C228" s="9"/>
       <c r="D228" s="9"/>
     </row>
-    <row r="229" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C229" s="9"/>
       <c r="D229" s="9"/>
     </row>
-    <row r="230" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C230" s="9"/>
       <c r="D230" s="9"/>
     </row>
-    <row r="231" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C231" s="9"/>
       <c r="D231" s="9"/>
     </row>
-    <row r="232" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C232" s="9"/>
       <c r="D232" s="9"/>
     </row>
-    <row r="233" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C233" s="9"/>
       <c r="D233" s="9"/>
     </row>
-    <row r="234" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C234" s="9"/>
       <c r="D234" s="9"/>
     </row>
-    <row r="235" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C235" s="9"/>
       <c r="D235" s="9"/>
     </row>
-    <row r="236" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C236" s="9"/>
       <c r="D236" s="9"/>
     </row>
-    <row r="237" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C237" s="9"/>
       <c r="D237" s="9"/>
     </row>
-    <row r="238" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C238" s="9"/>
       <c r="D238" s="9"/>
     </row>
-    <row r="239" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C239" s="9"/>
       <c r="D239" s="9"/>
     </row>
-    <row r="240" spans="3:4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C240" s="9"/>
       <c r="D240" s="9"/>
     </row>
@@ -3638,16 +5206,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:X1"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="AG1:AH1"/>
     <mergeCell ref="G1:K1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:X1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3659,7 +5227,7 @@
   <dimension ref="A1:AG110"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3852,36 +5420,36 @@
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="35" t="s">
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="35" t="s">
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="36"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="35" t="s">
+      <c r="L6" s="46"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="36"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="36" t="s">
+      <c r="O6" s="46"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="R6" s="36"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="36" t="s">
+      <c r="R6" s="46"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="U6" s="36"/>
-      <c r="V6" s="39"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="47"/>
       <c r="X6" s="26"/>
       <c r="Y6" s="26"/>
       <c r="Z6" s="26"/>
@@ -3898,24 +5466,24 @@
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="40"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="49"/>
       <c r="W7" s="26"/>
       <c r="X7" s="26"/>
       <c r="Y7" s="26"/>
@@ -3933,24 +5501,24 @@
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="43"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="33"/>
       <c r="W8" s="26"/>
       <c r="X8" s="26"/>
       <c r="Y8" s="26"/>
@@ -3968,24 +5536,24 @@
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="42"/>
-      <c r="V9" s="43"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="33"/>
       <c r="W9" s="26"/>
       <c r="X9" s="26"/>
       <c r="Y9" s="26"/>
@@ -4003,24 +5571,24 @@
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="V10" s="43"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="33"/>
       <c r="W10" s="26"/>
       <c r="X10" s="26"/>
       <c r="Y10" s="26"/>
@@ -4038,24 +5606,24 @@
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="43"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="33"/>
       <c r="W11" s="26"/>
       <c r="X11" s="26"/>
       <c r="Y11" s="26"/>
@@ -4073,24 +5641,24 @@
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="43"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="33"/>
       <c r="W12" s="26"/>
       <c r="X12" s="26"/>
       <c r="Y12" s="26"/>
@@ -4108,24 +5676,24 @@
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="42"/>
-      <c r="U13" s="42"/>
-      <c r="V13" s="43"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="33"/>
       <c r="W13" s="26"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
@@ -4143,24 +5711,24 @@
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="43"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="42"/>
-      <c r="V14" s="43"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="33"/>
       <c r="W14" s="26"/>
       <c r="X14" s="26"/>
       <c r="Y14" s="26"/>
@@ -4178,24 +5746,24 @@
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="43"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="42"/>
-      <c r="V15" s="43"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="33"/>
       <c r="W15" s="26"/>
       <c r="X15" s="26"/>
       <c r="Y15" s="26"/>
@@ -4213,24 +5781,24 @@
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="42"/>
-      <c r="V16" s="43"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="33"/>
       <c r="W16" s="26"/>
       <c r="X16" s="26"/>
       <c r="Y16" s="26"/>
@@ -4248,24 +5816,24 @@
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="42"/>
-      <c r="U17" s="42"/>
-      <c r="V17" s="43"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="33"/>
       <c r="W17" s="26"/>
       <c r="X17" s="26"/>
       <c r="Y17" s="26"/>
@@ -4283,24 +5851,24 @@
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="42"/>
-      <c r="U18" s="42"/>
-      <c r="V18" s="43"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="33"/>
       <c r="W18" s="26"/>
       <c r="X18" s="26"/>
       <c r="Y18" s="26"/>
@@ -4318,24 +5886,24 @@
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="43"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="42"/>
-      <c r="V19" s="43"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="33"/>
       <c r="W19" s="26"/>
       <c r="X19" s="26"/>
       <c r="Y19" s="26"/>
@@ -4353,24 +5921,24 @@
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="42"/>
-      <c r="U20" s="42"/>
-      <c r="V20" s="43"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="33"/>
       <c r="W20" s="26"/>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -4388,24 +5956,24 @@
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="42"/>
-      <c r="V21" s="43"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="33"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="33"/>
       <c r="W21" s="26"/>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -4423,24 +5991,24 @@
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="43"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="42"/>
-      <c r="V22" s="43"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="33"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="33"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
@@ -4458,24 +6026,24 @@
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="42"/>
-      <c r="U23" s="42"/>
-      <c r="V23" s="43"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="33"/>
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26"/>
@@ -4493,24 +6061,24 @@
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="43"/>
-      <c r="T24" s="42"/>
-      <c r="U24" s="42"/>
-      <c r="V24" s="43"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="32"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="33"/>
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26"/>
@@ -4528,24 +6096,24 @@
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="43"/>
-      <c r="T25" s="42"/>
-      <c r="U25" s="42"/>
-      <c r="V25" s="43"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="33"/>
       <c r="W25" s="26"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
@@ -4563,26 +6131,25 @@
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="43"/>
-      <c r="T26" s="42"/>
-      <c r="U26" s="42"/>
-      <c r="V26" s="43"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="32"/>
+      <c r="V26" s="33"/>
       <c r="W26" s="26"/>
-      <c r="X26" s="26"/>
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
       <c r="AA26" s="26"/>
@@ -4598,24 +6165,24 @@
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="42"/>
-      <c r="U27" s="42"/>
-      <c r="V27" s="43"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="33"/>
       <c r="W27" s="26"/>
       <c r="X27" s="26"/>
       <c r="Y27" s="26"/>
@@ -4633,28 +6200,27 @@
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="42"/>
-      <c r="U28" s="42"/>
-      <c r="V28" s="43"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="32"/>
+      <c r="U28" s="32"/>
+      <c r="V28" s="33"/>
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
       <c r="AA28" s="26"/>
       <c r="AB28" s="26"/>
       <c r="AC28" s="26"/>
@@ -4668,24 +6234,24 @@
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="42"/>
-      <c r="U29" s="42"/>
-      <c r="V29" s="43"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="33"/>
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
       <c r="Y29" s="26"/>
@@ -4703,24 +6269,24 @@
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="42"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="42"/>
-      <c r="U30" s="42"/>
-      <c r="V30" s="43"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="33"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="33"/>
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
@@ -4738,24 +6304,24 @@
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="42"/>
-      <c r="U31" s="42"/>
-      <c r="V31" s="43"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="33"/>
       <c r="W31" s="26"/>
       <c r="X31" s="26"/>
       <c r="Y31" s="26"/>
@@ -4773,24 +6339,24 @@
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="41"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="43"/>
-      <c r="T32" s="42"/>
-      <c r="U32" s="42"/>
-      <c r="V32" s="43"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="33"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="33"/>
       <c r="W32" s="26"/>
       <c r="X32" s="26"/>
       <c r="Y32" s="26"/>
@@ -4808,24 +6374,24 @@
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="42"/>
-      <c r="S33" s="43"/>
-      <c r="T33" s="42"/>
-      <c r="U33" s="42"/>
-      <c r="V33" s="43"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="33"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="33"/>
       <c r="W33" s="26"/>
       <c r="X33" s="26"/>
       <c r="Y33" s="26"/>
@@ -4843,24 +6409,24 @@
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="41"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="42"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="42"/>
-      <c r="U34" s="42"/>
-      <c r="V34" s="43"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="33"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="33"/>
       <c r="W34" s="26"/>
       <c r="X34" s="26"/>
     </row>
@@ -4869,24 +6435,24 @@
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="45"/>
-      <c r="P35" s="46"/>
-      <c r="Q35" s="45"/>
-      <c r="R35" s="45"/>
-      <c r="S35" s="46"/>
-      <c r="T35" s="45"/>
-      <c r="U35" s="45"/>
-      <c r="V35" s="46"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="36"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
+      <c r="S35" s="36"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="35"/>
+      <c r="V35" s="36"/>
       <c r="W35" s="26"/>
       <c r="X35" s="26"/>
     </row>
@@ -5566,7 +7132,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>